<commit_message>
Run bilat liquid period = 5d
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>CVA</t>
   </si>
@@ -45,9 +45,6 @@
     <t>KVA99</t>
   </si>
   <si>
-    <t>Bilat</t>
-  </si>
-  <si>
     <t>Ratio bilat / CCP</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>CCP (5 jours)</t>
+  </si>
+  <si>
+    <t>Bilat (15 jours)</t>
+  </si>
+  <si>
+    <t>Bilat (5 jours)</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,27 +521,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1"/>
       <c r="J3" s="1"/>
@@ -559,7 +562,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -727,21 +730,9 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -896,137 +887,388 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3">
-        <v>4.5380000000000004E-3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>9.2910000000000006E-3</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3">
-        <f>AVERAGE(D19,E19)</f>
-        <v>6.9145000000000005E-3</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="4">
-        <f>G19</f>
-        <v>6.9145000000000005E-3</v>
-      </c>
-      <c r="L19" s="1">
-        <f>I5/I19</f>
-        <v>4.7665051702943089</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1">
-        <v>6.783E-3</v>
-      </c>
-      <c r="E20" s="1">
-        <v>7.9780000000000007E-3</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <f>AVERAGE(D20,E20)</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="6">
-        <f t="shared" ref="I20:I23" si="3">G20</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" ref="L20:L23" si="4">I6/I20</f>
-        <v>3.9828602398211501</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <v>1.5200999999999999E-2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2.1562000000000001E-2</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1">
-        <f>AVERAGE(D21,E21)</f>
-        <v>1.8381500000000002E-2</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="6">
-        <f t="shared" si="3"/>
-        <v>1.8381500000000002E-2</v>
-      </c>
-      <c r="L21" s="1">
-        <f t="shared" si="4"/>
-        <v>2.2876261458531676E-2</v>
-      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3">
+        <v>3.4216999999999997E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3.5531E-2</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <f t="shared" ref="G21:G27" si="3">AVERAGE(D21,E21)</f>
+        <v>3.4874000000000002E-2</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="4">
+        <f>G21</f>
+        <v>3.4874000000000002E-2</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <v>5.4748999999999999E-2</v>
+        <v>3.2121999999999998E-2</v>
       </c>
       <c r="E22" s="1">
-        <v>5.6590000000000001E-2</v>
+        <v>3.3328999999999998E-2</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <f>AVERAGE(D22,E22)</f>
-        <v>5.5669499999999997E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.2725499999999998E-2</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="6">
+        <f t="shared" ref="I22:I23" si="4">G22</f>
+        <v>3.2725499999999998E-2</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <v>2.8E-5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.0499999999999998E-4</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
         <f t="shared" si="3"/>
+        <v>2.1649999999999998E-4</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="6">
+        <f t="shared" si="4"/>
+        <v>2.1649999999999998E-4</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <v>0.38505699999999998</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.40796700000000002</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <f t="shared" si="3"/>
+        <v>0.39651199999999998</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="6">
+        <f>SUM(G24,G26,)</f>
+        <v>0.52906750000000002</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <v>0.421126</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.44498500000000002</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.43305550000000004</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="6">
+        <f>SUM(G25,G27)</f>
+        <v>0.57880550000000008</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>0.12882199999999999</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.13628899999999999</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
+        <f t="shared" si="3"/>
+        <v>0.13255549999999999</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8">
+        <v>0.141843</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.14965700000000001</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8">
+        <f t="shared" si="3"/>
+        <v>0.14574999999999999</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <v>4.5380000000000004E-3</v>
+      </c>
+      <c r="E29" s="3">
+        <v>9.2910000000000006E-3</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3">
+        <f>AVERAGE(D29,E29)</f>
+        <v>6.9145000000000005E-3</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4">
+        <f>G29</f>
+        <v>6.9145000000000005E-3</v>
+      </c>
+      <c r="L29" s="1">
+        <f>I21/I29</f>
+        <v>5.043604020536554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1">
+        <v>6.783E-3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>7.9780000000000007E-3</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
+        <f>AVERAGE(D30,E30)</f>
+        <v>7.3804999999999999E-3</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="6">
+        <f t="shared" ref="I30:I33" si="5">G30</f>
+        <v>7.3804999999999999E-3</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" ref="L30:L33" si="6">I22/I30</f>
+        <v>4.434049183659643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <v>1.5200999999999999E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.1562000000000001E-2</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
+        <f>AVERAGE(D31,E31)</f>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="6">
+        <f t="shared" si="5"/>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1778146505997875E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1">
+        <v>5.4748999999999999E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5.6590000000000001E-2</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
+        <f>AVERAGE(D32,E32)</f>
         <v>5.5669499999999997E-2</v>
       </c>
-      <c r="L22" s="1">
-        <f t="shared" si="4"/>
-        <v>10.96432516907822</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="H32" s="1"/>
+      <c r="I32" s="6">
+        <f t="shared" si="5"/>
+        <v>5.5669499999999997E-2</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="6"/>
+        <v>9.5037228644051055</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8">
         <v>5.9089999999999997E-2</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E33" s="8">
         <v>6.0964999999999998E-2</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8">
-        <f>AVERAGE(D23,E23)</f>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8">
+        <f>AVERAGE(D33,E33)</f>
         <v>6.0027499999999998E-2</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="9">
-        <f t="shared" si="3"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="9">
+        <f t="shared" si="5"/>
         <v>6.0027499999999998E-2</v>
       </c>
-      <c r="L23" s="1">
-        <f t="shared" si="4"/>
-        <v>11.889508975053102</v>
-      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="6"/>
+        <v>9.6423389279913394</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New run with SA approach for KVA computation
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>CVA</t>
   </si>
@@ -57,9 +57,6 @@
     <t>moyenne</t>
   </si>
   <si>
-    <t>moyenne aggrégée</t>
-  </si>
-  <si>
     <t>1vs1</t>
   </si>
   <si>
@@ -73,6 +70,18 @@
   </si>
   <si>
     <t>Bilat (5 jours)</t>
+  </si>
+  <si>
+    <t>KVA_SA</t>
+  </si>
+  <si>
+    <t>moyenne aggrégée si besoin</t>
+  </si>
+  <si>
+    <t>KVA_CCR_SA</t>
+  </si>
+  <si>
+    <t>KVA_CVA_SA</t>
   </si>
 </sst>
 </file>
@@ -188,20 +197,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +539,7 @@
     <col min="1" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,8 +555,8 @@
         <v>12</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
+      <c r="I1" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -540,8 +564,8 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="11" t="s">
-        <v>14</v>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1"/>
       <c r="J3" s="1"/>
@@ -562,7 +586,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -580,7 +604,7 @@
         <v>3.2958000000000001E-2</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="4">
+      <c r="I5" s="13">
         <f>G5</f>
         <v>3.2958000000000001E-2</v>
       </c>
@@ -589,7 +613,7 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
@@ -605,7 +629,7 @@
         <v>2.9395499999999998E-2</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="6">
+      <c r="I6" s="12">
         <f t="shared" ref="I6:I7" si="1">G6</f>
         <v>2.9395499999999998E-2</v>
       </c>
@@ -614,7 +638,7 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1"/>
@@ -630,7 +654,7 @@
         <v>4.2050000000000003E-4</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="6">
+      <c r="I7" s="12">
         <f t="shared" si="1"/>
         <v>4.2050000000000003E-4</v>
       </c>
@@ -639,7 +663,7 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1"/>
@@ -655,8 +679,8 @@
         <v>0.45610399999999995</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="6">
-        <f>SUM(G8,G10,)</f>
+      <c r="I8" s="14">
+        <f>SUM(G8,G9,)</f>
         <v>0.61037849999999993</v>
       </c>
       <c r="J8" s="1"/>
@@ -664,75 +688,75 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>4</v>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <v>0.51880199999999999</v>
+        <v>0.15026200000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>0.54498199999999997</v>
+        <v>0.15828700000000001</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.53189200000000003</v>
+        <f>AVERAGE(D9,E9)</f>
+        <v>0.15427450000000001</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="6">
-        <f>SUM(G9,G11)</f>
-        <v>0.7136975000000001</v>
-      </c>
+      <c r="I9" s="14"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>5</v>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
-        <v>0.15026200000000001</v>
+        <v>0.51880199999999999</v>
       </c>
       <c r="E10" s="1">
-        <v>0.15828700000000001</v>
+        <v>0.54498199999999997</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.15427450000000001</v>
+        <f>AVERAGE(D10,E10)</f>
+        <v>0.53189200000000003</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="6"/>
+      <c r="I10" s="14">
+        <f>SUM(G10,G11)</f>
+        <v>0.7136975000000001</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
         <v>0.177458</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <v>0.18615300000000001</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
         <f t="shared" si="0"/>
         <v>0.18180550000000001</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -750,7 +774,7 @@
         <v>9.4914999999999999E-3</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="4">
+      <c r="I13" s="13">
         <f>G13</f>
         <v>9.4914999999999999E-3</v>
       </c>
@@ -762,7 +786,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1"/>
@@ -778,7 +802,7 @@
         <v>1.5802500000000001E-2</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="6">
+      <c r="I14" s="12">
         <f t="shared" ref="I14:I17" si="2">G14</f>
         <v>1.5802500000000001E-2</v>
       </c>
@@ -790,7 +814,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="1"/>
@@ -806,7 +830,7 @@
         <v>3.1036500000000002E-2</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="6">
+      <c r="I15" s="12">
         <f t="shared" si="2"/>
         <v>3.1036500000000002E-2</v>
       </c>
@@ -818,7 +842,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
@@ -834,7 +858,7 @@
         <v>6.1170000000000002E-2</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="6">
+      <c r="I16" s="12">
         <f t="shared" si="2"/>
         <v>6.1170000000000002E-2</v>
       </c>
@@ -846,30 +870,30 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6">
         <v>6.8559999999999996E-2</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>7.0557999999999996E-2</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6">
         <f>AVERAGE(D17,E17)</f>
         <v>6.9558999999999996E-2</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9">
+      <c r="H17" s="6"/>
+      <c r="I17" s="15">
         <f t="shared" si="2"/>
         <v>6.9558999999999996E-2</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1">
-        <f>I9/I17</f>
+        <f>I10/I17</f>
         <v>10.260318578472953</v>
       </c>
     </row>
@@ -914,7 +938,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
@@ -928,11 +952,11 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G27" si="3">AVERAGE(D21,E21)</f>
+        <f t="shared" ref="G21:G29" si="3">AVERAGE(D21,E21)</f>
         <v>3.4874000000000002E-2</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="4">
+      <c r="I21" s="13">
         <f>G21</f>
         <v>3.4874000000000002E-2</v>
       </c>
@@ -941,7 +965,7 @@
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
@@ -957,7 +981,7 @@
         <v>3.2725499999999998E-2</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="6">
+      <c r="I22" s="12">
         <f t="shared" ref="I22:I23" si="4">G22</f>
         <v>3.2725499999999998E-2</v>
       </c>
@@ -966,7 +990,7 @@
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="1"/>
@@ -982,7 +1006,7 @@
         <v>2.1649999999999998E-4</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="6">
+      <c r="I23" s="12">
         <f t="shared" si="4"/>
         <v>2.1649999999999998E-4</v>
       </c>
@@ -991,7 +1015,7 @@
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1"/>
@@ -1007,8 +1031,8 @@
         <v>0.39651199999999998</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="6">
-        <f>SUM(G24,G26,)</f>
+      <c r="I24" s="14">
+        <f>SUM(G24,G25,)</f>
         <v>0.52906750000000002</v>
       </c>
       <c r="J24" s="1"/>
@@ -1016,227 +1040,292 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>4</v>
+      <c r="B25" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>0.421126</v>
+        <v>0.12882199999999999</v>
       </c>
       <c r="E25" s="1">
-        <v>0.44498500000000002</v>
+        <v>0.13628899999999999</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
-        <f t="shared" si="3"/>
-        <v>0.43305550000000004</v>
+        <f>AVERAGE(D25,E25)</f>
+        <v>0.13255549999999999</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="6">
-        <f>SUM(G25,G27)</f>
-        <v>0.57880550000000008</v>
-      </c>
+      <c r="I25" s="14"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>5</v>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>0.12882199999999999</v>
+        <v>0.421126</v>
       </c>
       <c r="E26" s="1">
-        <v>0.13628899999999999</v>
+        <v>0.44498500000000002</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
-        <f t="shared" si="3"/>
-        <v>0.13255549999999999</v>
+        <f>AVERAGE(D26,E26)</f>
+        <v>0.43305550000000004</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="14">
+        <f>SUM(G26,G27)</f>
+        <v>0.57880550000000008</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1">
         <v>0.141843</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="1">
         <v>0.14965700000000001</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
         <f t="shared" si="3"/>
         <v>0.14574999999999999</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="9"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+      <c r="B28" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="7">
+        <v>0.30623400000000001</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.32685399999999998</v>
+      </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="7">
+        <f t="shared" ref="G28" si="5">AVERAGE(D28,E28)</f>
+        <v>0.31654399999999999</v>
+      </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="I28" s="14">
+        <f>SUM(G28:G29)</f>
+        <v>0.420427</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="11">
+        <v>0.100567</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.107199</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="11">
+        <f t="shared" si="3"/>
+        <v>0.103883</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
         <v>4.5380000000000004E-3</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E31" s="3">
         <v>9.2910000000000006E-3</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3">
-        <f>AVERAGE(D29,E29)</f>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
+        <f>AVERAGE(D31,E31)</f>
         <v>6.9145000000000005E-3</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="4">
-        <f>G29</f>
+      <c r="H31" s="3"/>
+      <c r="I31" s="13">
+        <f>G31</f>
         <v>6.9145000000000005E-3</v>
       </c>
-      <c r="L29" s="1">
-        <f>I21/I29</f>
+      <c r="L31" s="1">
+        <f>I21/I31</f>
         <v>5.043604020536554</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1">
-        <v>6.783E-3</v>
-      </c>
-      <c r="E30" s="1">
-        <v>7.9780000000000007E-3</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1">
-        <f>AVERAGE(D30,E30)</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="6">
-        <f t="shared" ref="I30:I33" si="5">G30</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="L30" s="1">
-        <f t="shared" ref="L30:L33" si="6">I22/I30</f>
-        <v>4.434049183659643</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1">
-        <v>1.5200999999999999E-2</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2.1562000000000001E-2</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1">
-        <f>AVERAGE(D31,E31)</f>
-        <v>1.8381500000000002E-2</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="6">
-        <f t="shared" si="5"/>
-        <v>1.8381500000000002E-2</v>
-      </c>
-      <c r="L31" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1778146505997875E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
-        <v>5.4748999999999999E-2</v>
+        <v>6.783E-3</v>
       </c>
       <c r="E32" s="1">
-        <v>5.6590000000000001E-2</v>
+        <v>7.9780000000000007E-3</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1">
         <f>AVERAGE(D32,E32)</f>
+        <v>7.3804999999999999E-3</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="12">
+        <f t="shared" ref="I32:I35" si="6">G32</f>
+        <v>7.3804999999999999E-3</v>
+      </c>
+      <c r="L32" s="1">
+        <f>I22/I32</f>
+        <v>4.434049183659643</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
+        <v>1.5200999999999999E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.1562000000000001E-2</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1">
+        <f>AVERAGE(D33,E33)</f>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="12">
+        <f t="shared" si="6"/>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="L33" s="1">
+        <f>I23/I33</f>
+        <v>1.1778146505997875E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <v>5.4748999999999999E-2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5.6590000000000001E-2</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
+        <f>AVERAGE(D34,E34)</f>
         <v>5.5669499999999997E-2</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="6">
-        <f t="shared" si="5"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="12">
+        <f t="shared" si="6"/>
         <v>5.5669499999999997E-2</v>
       </c>
-      <c r="L32" s="1">
+      <c r="L34" s="1">
+        <f>I24/I34</f>
+        <v>9.5037228644051055</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <v>5.9089999999999997E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6.0964999999999998E-2</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1">
+        <f>AVERAGE(D35,E35)</f>
+        <v>6.0027499999999998E-2</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="12">
         <f t="shared" si="6"/>
-        <v>9.5037228644051055</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8">
-        <v>5.9089999999999997E-2</v>
-      </c>
-      <c r="E33" s="8">
-        <v>6.0964999999999998E-2</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8">
-        <f>AVERAGE(D33,E33)</f>
         <v>6.0027499999999998E-2</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="9">
-        <f t="shared" si="5"/>
-        <v>6.0027499999999998E-2</v>
-      </c>
-      <c r="L33" s="1">
-        <f t="shared" si="6"/>
+      <c r="L35" s="1">
+        <f>I26/I35</f>
         <v>9.6423389279913394</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="B36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="11">
+        <v>4.5366999999999998E-2</v>
+      </c>
+      <c r="E36" s="11">
+        <v>4.7107000000000003E-2</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="11">
+        <f t="shared" ref="G36" si="7">AVERAGE(D36,E36)</f>
+        <v>4.6237E-2</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="15">
+        <f>G36</f>
+        <v>4.6237E-2</v>
+      </c>
+      <c r="L36" s="7">
+        <f>I28/I36</f>
+        <v>9.0928693470597146</v>
+      </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J37" s="1"/>
@@ -1259,18 +1348,33 @@
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added run with SA approach + results for liquid time = 15 days for both 1 vs 1
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>CVA</t>
   </si>
@@ -197,13 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -218,11 +217,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -528,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -564,7 +563,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1"/>
@@ -600,11 +599,11 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G11" si="0">AVERAGE(D5,E5)</f>
+        <f t="shared" ref="G5:G13" si="0">AVERAGE(D5,E5)</f>
         <v>3.2958000000000001E-2</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f>G5</f>
         <v>3.2958000000000001E-2</v>
       </c>
@@ -629,7 +628,7 @@
         <v>2.9395499999999998E-2</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <f t="shared" ref="I6:I7" si="1">G6</f>
         <v>2.9395499999999998E-2</v>
       </c>
@@ -654,7 +653,7 @@
         <v>4.2050000000000003E-4</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <f t="shared" si="1"/>
         <v>4.2050000000000003E-4</v>
       </c>
@@ -734,281 +733,291 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
         <v>0.177458</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="1">
         <v>0.18615300000000001</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>0.18180550000000001</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="16"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6">
+        <v>0.29057699999999997</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.31070700000000001</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.30064199999999996</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="14">
+        <f>SUM(G12:G13)</f>
+        <v>0.39890049999999999</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <v>6.0359999999999997E-3</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.2947E-2</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3">
-        <f>AVERAGE(D13,E13)</f>
-        <v>9.4914999999999999E-3</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="13">
-        <f>G13</f>
-        <v>9.4914999999999999E-3</v>
-      </c>
+      <c r="B13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="10">
+        <v>9.5032000000000005E-2</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.10148500000000001</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>9.8258499999999999E-2</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1">
-        <f>I5/I13</f>
-        <v>3.4723700152768266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
-        <v>1.4551E-2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1.7054E-2</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
-        <f>AVERAGE(D14,E14)</f>
-        <v>1.5802500000000001E-2</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="12">
-        <f t="shared" ref="I14:I17" si="2">G14</f>
-        <v>1.5802500000000001E-2</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1">
-        <f>I6/I14</f>
-        <v>1.8601803512102513</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1">
-        <v>2.792E-2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3.4153000000000003E-2</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
+        <v>6.0359999999999997E-3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.2947E-2</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
         <f>AVERAGE(D15,E15)</f>
-        <v>3.1036500000000002E-2</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>9.4914999999999999E-3</v>
+      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="12">
-        <f t="shared" si="2"/>
-        <v>3.1036500000000002E-2</v>
+        <f>G15</f>
+        <v>9.4914999999999999E-3</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1">
-        <f>I7/I15</f>
-        <v>1.3548563787798238E-2</v>
+        <f>I5/I15</f>
+        <v>3.4723700152768266</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
-        <v>6.0198000000000002E-2</v>
+        <v>1.4551E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>6.2142000000000003E-2</v>
+        <v>1.7054E-2</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
         <f>AVERAGE(D16,E16)</f>
-        <v>6.1170000000000002E-2</v>
+        <v>1.5802500000000001E-2</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="12">
-        <f t="shared" si="2"/>
-        <v>6.1170000000000002E-2</v>
+      <c r="I16" s="11">
+        <f t="shared" ref="I16:I19" si="2">G16</f>
+        <v>1.5802500000000001E-2</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1">
-        <f>I8/I16</f>
-        <v>9.9783962726826854</v>
+        <f>I6/I16</f>
+        <v>1.8601803512102513</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6">
-        <v>6.8559999999999996E-2</v>
-      </c>
-      <c r="E17" s="6">
-        <v>7.0557999999999996E-2</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6">
+      <c r="B17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>2.792E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.4153000000000003E-2</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
         <f>AVERAGE(D17,E17)</f>
-        <v>6.9558999999999996E-2</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="15">
+        <v>3.1036500000000002E-2</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="11">
         <f t="shared" si="2"/>
-        <v>6.9558999999999996E-2</v>
+        <v>3.1036500000000002E-2</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1">
-        <f>I10/I17</f>
-        <v>10.260318578472953</v>
+        <f>I7/I17</f>
+        <v>1.3548563787798238E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1">
+        <v>6.0198000000000002E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6.2142000000000003E-2</v>
+      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1">
+        <f>AVERAGE(D18,E18)</f>
+        <v>6.1170000000000002E-2</v>
+      </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="11">
+        <f t="shared" si="2"/>
+        <v>6.1170000000000002E-2</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <f>I8/I18</f>
+        <v>9.9783962726826854</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1">
+        <v>6.8559999999999996E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7.0557999999999996E-2</v>
+      </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1">
+        <f>AVERAGE(D19,E19)</f>
+        <v>6.9558999999999996E-2</v>
+      </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="11">
+        <f t="shared" si="2"/>
+        <v>6.9558999999999996E-2</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <f>I10/I19</f>
+        <v>10.260318578472953</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="B20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="10">
+        <v>4.3317000000000001E-2</v>
+      </c>
+      <c r="E20" s="10">
+        <v>4.5073000000000002E-2</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="10">
+        <f t="shared" ref="G20" si="3">AVERAGE(D20,E20)</f>
+        <v>4.4194999999999998E-2</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="13">
+        <f>G20</f>
+        <v>4.4194999999999998E-2</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1">
+        <f>I12/I20</f>
+        <v>9.0259192216314066</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <v>3.4216999999999997E-2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>3.5531E-2</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3">
-        <f t="shared" ref="G21:G29" si="3">AVERAGE(D21,E21)</f>
-        <v>3.4874000000000002E-2</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="13">
-        <f>G21</f>
-        <v>3.4874000000000002E-2</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1">
-        <v>3.2121999999999998E-2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>3.3328999999999998E-2</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1">
-        <f t="shared" si="3"/>
-        <v>3.2725499999999998E-2</v>
-      </c>
+      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="12">
-        <f t="shared" ref="I22:I23" si="4">G22</f>
-        <v>3.2725499999999998E-2</v>
-      </c>
+      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1">
-        <v>2.8E-5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>4.0499999999999998E-4</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
-        <f t="shared" si="3"/>
-        <v>2.1649999999999998E-4</v>
-      </c>
-      <c r="H23" s="1"/>
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
+        <v>3.4216999999999997E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3.5531E-2</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3">
+        <f t="shared" ref="G23:G31" si="4">AVERAGE(D23,E23)</f>
+        <v>3.4874000000000002E-2</v>
+      </c>
+      <c r="H23" s="3"/>
       <c r="I23" s="12">
-        <f t="shared" si="4"/>
-        <v>2.1649999999999998E-4</v>
+        <f>G23</f>
+        <v>3.4874000000000002E-2</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1016,24 +1025,24 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
-        <v>0.38505699999999998</v>
+        <v>3.2121999999999998E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>0.40796700000000002</v>
+        <v>3.3328999999999998E-2</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1">
-        <f t="shared" si="3"/>
-        <v>0.39651199999999998</v>
+        <f t="shared" si="4"/>
+        <v>3.2725499999999998E-2</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="14">
-        <f>SUM(G24,G25,)</f>
-        <v>0.52906750000000002</v>
+      <c r="I24" s="11">
+        <f t="shared" ref="I24:I25" si="5">G24</f>
+        <v>3.2725499999999998E-2</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1041,46 +1050,49 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>0.12882199999999999</v>
+        <v>2.8E-5</v>
       </c>
       <c r="E25" s="1">
-        <v>0.13628899999999999</v>
+        <v>4.0499999999999998E-4</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
-        <f>AVERAGE(D25,E25)</f>
-        <v>0.13255549999999999</v>
+        <f t="shared" si="4"/>
+        <v>2.1649999999999998E-4</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="14"/>
+      <c r="I25" s="11">
+        <f t="shared" si="5"/>
+        <v>2.1649999999999998E-4</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>0.421126</v>
+        <v>0.38505699999999998</v>
       </c>
       <c r="E26" s="1">
-        <v>0.44498500000000002</v>
+        <v>0.40796700000000002</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
-        <f>AVERAGE(D26,E26)</f>
-        <v>0.43305550000000004</v>
+        <f t="shared" si="4"/>
+        <v>0.39651199999999998</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="14">
-        <f>SUM(G26,G27)</f>
-        <v>0.57880550000000008</v>
+        <f>SUM(G26,G27,)</f>
+        <v>0.52906750000000002</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1088,19 +1100,19 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>0.141843</v>
+        <v>0.12882199999999999</v>
       </c>
       <c r="E27" s="1">
-        <v>0.14965700000000001</v>
+        <v>0.13628899999999999</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
-        <f t="shared" si="3"/>
-        <v>0.14574999999999999</v>
+        <f>AVERAGE(D27,E27)</f>
+        <v>0.13255549999999999</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="14"/>
@@ -1109,271 +1121,319 @@
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
-        <v>20</v>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="7">
-        <v>0.30623400000000001</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0.32685399999999998</v>
+      <c r="D28" s="1">
+        <v>0.421126</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.44498500000000002</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="7">
-        <f t="shared" ref="G28" si="5">AVERAGE(D28,E28)</f>
-        <v>0.31654399999999999</v>
+      <c r="G28" s="1">
+        <f>AVERAGE(D28,E28)</f>
+        <v>0.43305550000000004</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="14">
-        <f>SUM(G28:G29)</f>
-        <v>0.420427</v>
+        <f>SUM(G28,G29)</f>
+        <v>0.57880550000000008</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11">
-        <v>0.100567</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.107199</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="11">
-        <f t="shared" si="3"/>
-        <v>0.103883</v>
-      </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="16"/>
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <v>0.141843</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.14965700000000001</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
+        <f t="shared" si="4"/>
+        <v>0.14574999999999999</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+      <c r="B30" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="6">
+        <v>0.30623400000000001</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.32685399999999998</v>
+      </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="6">
+        <f t="shared" ref="G30" si="6">AVERAGE(D30,E30)</f>
+        <v>0.31654399999999999</v>
+      </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="I30" s="14">
+        <f>SUM(G30:G31)</f>
+        <v>0.420427</v>
+      </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="10">
+        <v>0.100567</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0.107199</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="10">
+        <f t="shared" si="4"/>
+        <v>0.103883</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3">
         <v>4.5380000000000004E-3</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E33" s="3">
         <v>9.2910000000000006E-3</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3">
-        <f>AVERAGE(D31,E31)</f>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3">
+        <f>AVERAGE(D33,E33)</f>
         <v>6.9145000000000005E-3</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="13">
-        <f>G31</f>
+      <c r="H33" s="3"/>
+      <c r="I33" s="12">
+        <f>G33</f>
         <v>6.9145000000000005E-3</v>
-      </c>
-      <c r="L31" s="1">
-        <f>I21/I31</f>
-        <v>5.043604020536554</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1">
-        <v>6.783E-3</v>
-      </c>
-      <c r="E32" s="1">
-        <v>7.9780000000000007E-3</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1">
-        <f>AVERAGE(D32,E32)</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="12">
-        <f t="shared" ref="I32:I35" si="6">G32</f>
-        <v>7.3804999999999999E-3</v>
-      </c>
-      <c r="L32" s="1">
-        <f>I22/I32</f>
-        <v>4.434049183659643</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1">
-        <v>1.5200999999999999E-2</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2.1562000000000001E-2</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1">
-        <f>AVERAGE(D33,E33)</f>
-        <v>1.8381500000000002E-2</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="12">
-        <f t="shared" si="6"/>
-        <v>1.8381500000000002E-2</v>
       </c>
       <c r="L33" s="1">
         <f>I23/I33</f>
-        <v>1.1778146505997875E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+        <v>5.043604020536554</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>5.4748999999999999E-2</v>
+        <v>6.783E-3</v>
       </c>
       <c r="E34" s="1">
-        <v>5.6590000000000001E-2</v>
+        <v>7.9780000000000007E-3</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1">
         <f>AVERAGE(D34,E34)</f>
-        <v>5.5669499999999997E-2</v>
+        <v>7.3804999999999999E-3</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="12">
-        <f t="shared" si="6"/>
-        <v>5.5669499999999997E-2</v>
+      <c r="I34" s="11">
+        <f t="shared" ref="I34:I37" si="7">G34</f>
+        <v>7.3804999999999999E-3</v>
       </c>
       <c r="L34" s="1">
         <f>I24/I34</f>
-        <v>9.5037228644051055</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+        <v>4.434049183659643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
-        <v>5.9089999999999997E-2</v>
+        <v>1.5200999999999999E-2</v>
       </c>
       <c r="E35" s="1">
-        <v>6.0964999999999998E-2</v>
+        <v>2.1562000000000001E-2</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1">
         <f>AVERAGE(D35,E35)</f>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="11">
+        <f t="shared" si="7"/>
+        <v>1.8381500000000002E-2</v>
+      </c>
+      <c r="L35" s="1">
+        <f>I25/I35</f>
+        <v>1.1778146505997875E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1">
+        <v>5.4748999999999999E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5.6590000000000001E-2</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1">
+        <f>AVERAGE(D36,E36)</f>
+        <v>5.5669499999999997E-2</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="11">
+        <f t="shared" si="7"/>
+        <v>5.5669499999999997E-2</v>
+      </c>
+      <c r="L36" s="1">
+        <f>I26/I36</f>
+        <v>9.5037228644051055</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1">
+        <v>5.9089999999999997E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>6.0964999999999998E-2</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1">
+        <f>AVERAGE(D37,E37)</f>
         <v>6.0027499999999998E-2</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="12">
-        <f t="shared" si="6"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="11">
+        <f t="shared" si="7"/>
         <v>6.0027499999999998E-2</v>
       </c>
-      <c r="L35" s="1">
-        <f>I26/I35</f>
+      <c r="L37" s="1">
+        <f>I28/I37</f>
         <v>9.6423389279913394</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="11">
+      <c r="C38" s="5"/>
+      <c r="D38" s="10">
         <v>4.5366999999999998E-2</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E38" s="10">
         <v>4.7107000000000003E-2</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="11">
-        <f t="shared" ref="G36" si="7">AVERAGE(D36,E36)</f>
+      <c r="F38" s="5"/>
+      <c r="G38" s="10">
+        <f t="shared" ref="G38" si="8">AVERAGE(D38,E38)</f>
         <v>4.6237E-2</v>
       </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="15">
-        <f>G36</f>
+      <c r="H38" s="5"/>
+      <c r="I38" s="13">
+        <f>G38</f>
         <v>4.6237E-2</v>
       </c>
-      <c r="L36" s="7">
-        <f>I28/I36</f>
+      <c r="L38" s="6">
+        <f>I30/I38</f>
         <v>9.0928693470597146</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I24:I25"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Run with SA approach + results for liquid time = 15 days for all 1 vs 60
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
   <si>
     <t>CVA</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>KVA99</t>
-  </si>
-  <si>
-    <t>Ratio bilat / CCP</t>
   </si>
   <si>
     <t>borne inf</t>
@@ -107,18 +104,33 @@
   <si>
     <t>G5-G4</t>
   </si>
+  <si>
+    <t>1vs60</t>
+  </si>
+  <si>
+    <t>Ratio CCP / bilat</t>
+  </si>
+  <si>
+    <t>Ratio Bilat / CCP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -301,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -357,6 +369,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S80"/>
+  <dimension ref="B1:S143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S116" sqref="S116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,32 +690,35 @@
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -742,7 +760,7 @@
       <c r="E4" s="18"/>
       <c r="F4" s="1"/>
       <c r="G4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -782,7 +800,7 @@
       <c r="E6" s="18"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>0</v>
@@ -996,7 +1014,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
       <c r="H13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="6">
@@ -1027,7 +1045,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="20"/>
       <c r="H14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="8">
@@ -1073,7 +1091,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>0</v>
@@ -1100,7 +1118,10 @@
         <f>O6/O16</f>
         <v>3.4723700152768266</v>
       </c>
-      <c r="R16" s="15"/>
+      <c r="R16" s="15">
+        <f>1/Q16</f>
+        <v>0.28798774197463439</v>
+      </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
@@ -1134,7 +1155,10 @@
         <f>O7/O17</f>
         <v>1.8601803512102513</v>
       </c>
-      <c r="R17" s="15"/>
+      <c r="R17" s="15">
+        <f t="shared" ref="R17:R21" si="3">1/Q17</f>
+        <v>0.53758228300250044</v>
+      </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
@@ -1168,7 +1192,10 @@
         <f>O8/O18</f>
         <v>1.3548563787798238E-2</v>
       </c>
-      <c r="R18" s="15"/>
+      <c r="R18" s="15">
+        <f t="shared" si="3"/>
+        <v>73.808561236623063</v>
+      </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
@@ -1202,7 +1229,10 @@
         <f>O9/O19</f>
         <v>9.9783962726826854</v>
       </c>
-      <c r="R19" s="15"/>
+      <c r="R19" s="15">
+        <f t="shared" si="3"/>
+        <v>0.10021650500468154</v>
+      </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
@@ -1236,7 +1266,10 @@
         <f>O11/O20</f>
         <v>10.260318578472953</v>
       </c>
-      <c r="R20" s="15"/>
+      <c r="R20" s="15">
+        <f t="shared" si="3"/>
+        <v>9.7462860665758239E-2</v>
+      </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
@@ -1246,7 +1279,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="20"/>
       <c r="H21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="8">
@@ -1257,7 +1290,7 @@
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="8">
-        <f t="shared" ref="M21" si="3">AVERAGE(J21,K21)</f>
+        <f t="shared" ref="M21" si="4">AVERAGE(J21,K21)</f>
         <v>4.4194999999999998E-2</v>
       </c>
       <c r="N21" s="5"/>
@@ -1270,7 +1303,10 @@
         <f>O13/O21</f>
         <v>9.0259192216314066</v>
       </c>
-      <c r="R21" s="15"/>
+      <c r="R21" s="15">
+        <f t="shared" si="3"/>
+        <v>0.11079203961890245</v>
+      </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
@@ -1317,7 +1353,7 @@
       <c r="E24" s="18"/>
       <c r="F24" s="1"/>
       <c r="G24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>0</v>
@@ -1331,7 +1367,7 @@
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3">
-        <f t="shared" ref="M24:M32" si="4">AVERAGE(J24,K24)</f>
+        <f t="shared" ref="M24:M32" si="5">AVERAGE(J24,K24)</f>
         <v>3.4874000000000002E-2</v>
       </c>
       <c r="N24" s="3"/>
@@ -1362,12 +1398,12 @@
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2725499999999998E-2</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="9">
-        <f t="shared" ref="O25:O26" si="5">M25</f>
+        <f t="shared" ref="O25:O26" si="6">M25</f>
         <v>3.2725499999999998E-2</v>
       </c>
       <c r="P25" s="1"/>
@@ -1393,12 +1429,12 @@
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1649999999999998E-4</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1649999999999998E-4</v>
       </c>
       <c r="P26" s="1"/>
@@ -1424,7 +1460,7 @@
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.39651199999999998</v>
       </c>
       <c r="N27" s="1"/>
@@ -1514,7 +1550,7 @@
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14574999999999999</v>
       </c>
       <c r="N30" s="1"/>
@@ -1531,7 +1567,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="4"/>
       <c r="H31" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="6">
@@ -1542,7 +1578,7 @@
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="6">
-        <f t="shared" ref="M31" si="6">AVERAGE(J31,K31)</f>
+        <f t="shared" ref="M31" si="7">AVERAGE(J31,K31)</f>
         <v>0.31654399999999999</v>
       </c>
       <c r="N31" s="1"/>
@@ -1562,7 +1598,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="20"/>
       <c r="H32" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="8">
@@ -1573,7 +1609,7 @@
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.103883</v>
       </c>
       <c r="N32" s="5"/>
@@ -1608,7 +1644,7 @@
       <c r="E34" s="18"/>
       <c r="F34" s="1"/>
       <c r="G34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>0</v>
@@ -1635,7 +1671,10 @@
         <f>O24/O34</f>
         <v>5.043604020536554</v>
       </c>
-      <c r="R34" s="15"/>
+      <c r="R34" s="15">
+        <f>1/Q34</f>
+        <v>0.19827091816252795</v>
+      </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="22"/>
@@ -1661,7 +1700,7 @@
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="9">
-        <f t="shared" ref="O35:O38" si="7">M35</f>
+        <f t="shared" ref="O35:O38" si="8">M35</f>
         <v>7.3804999999999999E-3</v>
       </c>
       <c r="P35" s="1"/>
@@ -1669,7 +1708,10 @@
         <f>O25/O35</f>
         <v>4.434049183659643</v>
       </c>
-      <c r="R35" s="15"/>
+      <c r="R35" s="15">
+        <f t="shared" ref="R35:R39" si="9">1/Q35</f>
+        <v>0.22552749385036139</v>
+      </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" s="22"/>
@@ -1695,7 +1737,7 @@
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8381500000000002E-2</v>
       </c>
       <c r="P36" s="1"/>
@@ -1703,7 +1745,10 @@
         <f>O26/O36</f>
         <v>1.1778146505997875E-2</v>
       </c>
-      <c r="R36" s="15"/>
+      <c r="R36" s="15">
+        <f t="shared" si="9"/>
+        <v>84.903002309468846</v>
+      </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" s="22"/>
@@ -1729,7 +1774,7 @@
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.5669499999999997E-2</v>
       </c>
       <c r="P37" s="1"/>
@@ -1737,7 +1782,10 @@
         <f>O27/O37</f>
         <v>9.5037228644051055</v>
       </c>
-      <c r="R37" s="15"/>
+      <c r="R37" s="15">
+        <f t="shared" si="9"/>
+        <v>0.10522192347857315</v>
+      </c>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
@@ -1763,7 +1811,7 @@
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.0027499999999998E-2</v>
       </c>
       <c r="P38" s="1"/>
@@ -1771,7 +1819,10 @@
         <f>O29/O38</f>
         <v>9.6423389279913394</v>
       </c>
-      <c r="R38" s="15"/>
+      <c r="R38" s="15">
+        <f t="shared" si="9"/>
+        <v>0.10370927712331687</v>
+      </c>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" s="22"/>
@@ -1781,7 +1832,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="20"/>
       <c r="H39" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="8">
@@ -1792,7 +1843,7 @@
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="8">
-        <f t="shared" ref="M39" si="8">AVERAGE(J39,K39)</f>
+        <f t="shared" ref="M39" si="10">AVERAGE(J39,K39)</f>
         <v>4.6237E-2</v>
       </c>
       <c r="N39" s="5"/>
@@ -1805,7 +1856,10 @@
         <f>O31/O39</f>
         <v>9.0928693470597146</v>
       </c>
-      <c r="R39" s="15"/>
+      <c r="R39" s="15">
+        <f t="shared" si="9"/>
+        <v>0.10997628601398102</v>
+      </c>
     </row>
     <row r="40" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="23"/>
@@ -1881,17 +1935,17 @@
         <v>80</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="18">
         <v>38</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1912,7 +1966,7 @@
         <v>104</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1935,11 +1989,11 @@
         <v>76</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>0</v>
@@ -1953,7 +2007,7 @@
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3">
-        <f t="shared" ref="M46:M49" si="9">AVERAGE(J46,K46)</f>
+        <f t="shared" ref="M46:M49" si="11">AVERAGE(J46,K46)</f>
         <v>1.1450659999999999</v>
       </c>
       <c r="N46" s="3"/>
@@ -1972,7 +2026,7 @@
         <v>120</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="4"/>
@@ -1988,12 +2042,12 @@
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.43753350000000002</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="9">
-        <f t="shared" ref="O47:O48" si="10">M47</f>
+        <f t="shared" ref="O47:O48" si="12">M47</f>
         <v>0.43753350000000002</v>
       </c>
       <c r="P47" s="1"/>
@@ -2007,7 +2061,7 @@
         <v>50</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="4"/>
@@ -2023,12 +2077,12 @@
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.195E-4</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.195E-4</v>
       </c>
       <c r="P48" s="1"/>
@@ -2042,7 +2096,7 @@
         <v>107</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="4"/>
@@ -2058,7 +2112,7 @@
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.57179449999999998</v>
       </c>
       <c r="N49" s="1"/>
@@ -2077,7 +2131,7 @@
         <v>61</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="4"/>
@@ -2109,7 +2163,7 @@
         <v>87</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="4"/>
@@ -2144,7 +2198,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="4"/>
@@ -2160,7 +2214,7 @@
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1">
-        <f t="shared" ref="M52:M54" si="11">AVERAGE(J52,K52)</f>
+        <f t="shared" ref="M52:M54" si="13">AVERAGE(J52,K52)</f>
         <v>0.75662399999999996</v>
       </c>
       <c r="N52" s="1"/>
@@ -2176,12 +2230,12 @@
         <v>34</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="4"/>
       <c r="H53" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="6">
@@ -2192,7 +2246,7 @@
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.37829049999999997</v>
       </c>
       <c r="N53" s="1"/>
@@ -2212,7 +2266,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="20"/>
       <c r="H54" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="8">
@@ -2223,7 +2277,7 @@
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.40857450000000001</v>
       </c>
       <c r="N54" s="5"/>
@@ -2258,7 +2312,7 @@
       <c r="E56" s="18"/>
       <c r="F56" s="1"/>
       <c r="G56" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>0</v>
@@ -2285,7 +2339,10 @@
         <f>O46/O56</f>
         <v>35.923639215686272</v>
       </c>
-      <c r="R56" s="15"/>
+      <c r="R56" s="15">
+        <f>1/Q56</f>
+        <v>2.7836823379613056E-2</v>
+      </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="22"/>
@@ -2311,7 +2368,7 @@
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="9">
-        <f t="shared" ref="O57:O60" si="12">M57</f>
+        <f t="shared" ref="O57:O60" si="14">M57</f>
         <v>2.0728E-2</v>
       </c>
       <c r="P57" s="1"/>
@@ -2319,7 +2376,10 @@
         <f>O47/O57</f>
         <v>21.108331725202625</v>
       </c>
-      <c r="R57" s="15"/>
+      <c r="R57" s="15">
+        <f t="shared" ref="R57:R61" si="15">1/Q57</f>
+        <v>4.7374658169031629E-2</v>
+      </c>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="22"/>
@@ -2345,7 +2405,7 @@
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.6397499999999999E-2</v>
       </c>
       <c r="P58" s="1"/>
@@ -2353,7 +2413,10 @@
         <f>O48/O58</f>
         <v>1.4272958307576069E-2</v>
       </c>
-      <c r="R58" s="15"/>
+      <c r="R58" s="15">
+        <f t="shared" si="15"/>
+        <v>70.062560153994227</v>
+      </c>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="22"/>
@@ -2379,7 +2442,7 @@
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.1149999999999996E-2</v>
       </c>
       <c r="P59" s="1"/>
@@ -2387,7 +2450,10 @@
         <f>O49/O59</f>
         <v>19.848315617334425</v>
       </c>
-      <c r="R59" s="15"/>
+      <c r="R59" s="15">
+        <f t="shared" si="15"/>
+        <v>5.0382108954709244E-2</v>
+      </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="22"/>
@@ -2413,7 +2479,7 @@
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.9530000000000008E-2</v>
       </c>
       <c r="P60" s="1"/>
@@ -2421,7 +2487,10 @@
         <f>O51/O60</f>
         <v>20.461103120954981</v>
       </c>
-      <c r="R60" s="15"/>
+      <c r="R60" s="15">
+        <f t="shared" si="15"/>
+        <v>4.8873220279891098E-2</v>
+      </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="22"/>
@@ -2431,7 +2500,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="20"/>
       <c r="H61" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="8">
@@ -2442,7 +2511,7 @@
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="8">
-        <f t="shared" ref="M61" si="13">AVERAGE(J61,K61)</f>
+        <f t="shared" ref="M61" si="16">AVERAGE(J61,K61)</f>
         <v>4.4184500000000002E-2</v>
       </c>
       <c r="N61" s="5"/>
@@ -2455,7 +2524,10 @@
         <f>O53/O61</f>
         <v>17.808620670144506</v>
       </c>
-      <c r="R61" s="15"/>
+      <c r="R61" s="15">
+        <f t="shared" si="15"/>
+        <v>5.6152580175760775E-2</v>
+      </c>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="22"/>
@@ -2502,7 +2574,7 @@
       <c r="E64" s="18"/>
       <c r="F64" s="1"/>
       <c r="G64" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>0</v>
@@ -2516,7 +2588,7 @@
       </c>
       <c r="L64" s="3"/>
       <c r="M64" s="3">
-        <f t="shared" ref="M64:M67" si="14">AVERAGE(J64,K64)</f>
+        <f t="shared" ref="M64:M67" si="17">AVERAGE(J64,K64)</f>
         <v>1.152155</v>
       </c>
       <c r="N64" s="3"/>
@@ -2547,12 +2619,12 @@
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.44150149999999999</v>
       </c>
       <c r="N65" s="1"/>
       <c r="O65" s="9">
-        <f t="shared" ref="O65:O66" si="15">M65</f>
+        <f t="shared" ref="O65:O66" si="18">M65</f>
         <v>0.44150149999999999</v>
       </c>
       <c r="P65" s="1"/>
@@ -2578,12 +2650,12 @@
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>2.9700000000000001E-4</v>
       </c>
       <c r="N66" s="1"/>
       <c r="O66" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>2.9700000000000001E-4</v>
       </c>
       <c r="P66" s="1"/>
@@ -2609,7 +2681,7 @@
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.4977125</v>
       </c>
       <c r="N67" s="1"/>
@@ -2699,7 +2771,7 @@
       </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1">
-        <f t="shared" ref="M70:M72" si="16">AVERAGE(J70,K70)</f>
+        <f t="shared" ref="M70:M72" si="19">AVERAGE(J70,K70)</f>
         <v>0.60645300000000002</v>
       </c>
       <c r="N70" s="1"/>
@@ -2716,7 +2788,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="4"/>
       <c r="H71" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="6">
@@ -2727,7 +2799,7 @@
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.39807099999999995</v>
       </c>
       <c r="N71" s="1"/>
@@ -2747,7 +2819,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="20"/>
       <c r="H72" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="8">
@@ -2758,7 +2830,7 @@
       </c>
       <c r="L72" s="5"/>
       <c r="M72" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.4319925</v>
       </c>
       <c r="N72" s="5"/>
@@ -2793,7 +2865,7 @@
       <c r="E74" s="18"/>
       <c r="F74" s="1"/>
       <c r="G74" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>0</v>
@@ -2820,7 +2892,10 @@
         <f>O64/O74</f>
         <v>50.988206138118741</v>
       </c>
-      <c r="R74" s="15"/>
+      <c r="R74" s="15">
+        <f>1/Q74</f>
+        <v>1.9612378542817586E-2</v>
+      </c>
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="22"/>
@@ -2846,7 +2921,7 @@
       </c>
       <c r="N75" s="1"/>
       <c r="O75" s="9">
-        <f t="shared" ref="O75:O78" si="17">M75</f>
+        <f t="shared" ref="O75:O78" si="20">M75</f>
         <v>9.604999999999999E-3</v>
       </c>
       <c r="P75" s="1"/>
@@ -2854,7 +2929,10 @@
         <f>O65/O75</f>
         <v>45.965799062988033</v>
       </c>
-      <c r="R75" s="15"/>
+      <c r="R75" s="15">
+        <f t="shared" ref="R75:R79" si="21">1/Q75</f>
+        <v>2.1755305474613334E-2</v>
+      </c>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="22"/>
@@ -2880,7 +2958,7 @@
       </c>
       <c r="N76" s="1"/>
       <c r="O76" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2.1894999999999998E-2</v>
       </c>
       <c r="P76" s="1"/>
@@ -2888,7 +2966,10 @@
         <f>O66/O76</f>
         <v>1.3564740808403747E-2</v>
       </c>
-      <c r="R76" s="15"/>
+      <c r="R76" s="15">
+        <f t="shared" si="21"/>
+        <v>73.720538720538713</v>
+      </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="22"/>
@@ -2914,7 +2995,7 @@
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.57005E-2</v>
       </c>
       <c r="P77" s="1"/>
@@ -2922,7 +3003,10 @@
         <f>O67/O77</f>
         <v>18.836114577068425</v>
       </c>
-      <c r="R77" s="15"/>
+      <c r="R77" s="15">
+        <f t="shared" si="21"/>
+        <v>5.3089505052035836E-2</v>
+      </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="22"/>
@@ -2948,7 +3032,7 @@
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6.0058500000000001E-2</v>
       </c>
       <c r="P78" s="1"/>
@@ -2956,7 +3040,10 @@
         <f>O69/O78</f>
         <v>19.142277945669637</v>
       </c>
-      <c r="R78" s="15"/>
+      <c r="R78" s="15">
+        <f t="shared" si="21"/>
+        <v>5.2240386585036491E-2</v>
+      </c>
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="22"/>
@@ -2966,7 +3053,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="20"/>
       <c r="H79" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="8">
@@ -2977,7 +3064,7 @@
       </c>
       <c r="L79" s="5"/>
       <c r="M79" s="8">
-        <f t="shared" ref="M79" si="18">AVERAGE(J79,K79)</f>
+        <f t="shared" ref="M79" si="22">AVERAGE(J79,K79)</f>
         <v>4.6269000000000005E-2</v>
       </c>
       <c r="N79" s="5"/>
@@ -2990,7 +3077,10 @@
         <f>O71/O79</f>
         <v>17.939948993926816</v>
       </c>
-      <c r="R79" s="15"/>
+      <c r="R79" s="15">
+        <f t="shared" si="21"/>
+        <v>5.5741518570567201E-2</v>
+      </c>
     </row>
     <row r="80" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="23"/>
@@ -3011,8 +3101,1660 @@
       <c r="Q80" s="16"/>
       <c r="R80" s="17"/>
     </row>
+    <row r="82" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B83" s="12"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
+      <c r="O83" s="13"/>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="13"/>
+      <c r="R83" s="14"/>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B84" s="22">
+        <v>80</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="18">
+        <v>3</v>
+      </c>
+      <c r="E84" s="18"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="15"/>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B85" s="22"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18">
+        <v>4</v>
+      </c>
+      <c r="E85" s="18"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="15"/>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B86" s="22"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18">
+        <v>5</v>
+      </c>
+      <c r="E86" s="18"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3" t="e">
+        <f t="shared" ref="M86:M89" si="23">AVERAGE(J86,K86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N86" s="3"/>
+      <c r="O86" s="10" t="e">
+        <f>M86</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="15"/>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B87" s="22"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18">
+        <v>9</v>
+      </c>
+      <c r="E87" s="25"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N87" s="1"/>
+      <c r="O87" s="9" t="e">
+        <f t="shared" ref="O87:O88" si="24">M87</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="15"/>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B88" s="22"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18">
+        <v>13</v>
+      </c>
+      <c r="E88" s="25"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N88" s="1"/>
+      <c r="O88" s="9" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="15"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B89" s="22"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18">
+        <v>17</v>
+      </c>
+      <c r="E89" s="25"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I89" s="1"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N89" s="1"/>
+      <c r="O89" s="26" t="e">
+        <f>SUM(M89,M90,)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="15"/>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B90" s="22"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18">
+        <v>24</v>
+      </c>
+      <c r="E90" s="25"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I90" s="1"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1" t="e">
+        <f>AVERAGE(J90,K90)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N90" s="1"/>
+      <c r="O90" s="26"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="15"/>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B91" s="22"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18">
+        <v>25</v>
+      </c>
+      <c r="E91" s="25"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I91" s="1"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1" t="e">
+        <f>AVERAGE(J91,K91)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N91" s="1"/>
+      <c r="O91" s="26" t="e">
+        <f>SUM(M91,M92)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="15"/>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B92" s="22"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18">
+        <v>26</v>
+      </c>
+      <c r="E92" s="25"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I92" s="1"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1" t="e">
+        <f t="shared" ref="M92:M94" si="25">AVERAGE(J92,K92)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N92" s="1"/>
+      <c r="O92" s="26"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="15"/>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B93" s="22"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18">
+        <v>27</v>
+      </c>
+      <c r="E93" s="25"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="6" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N93" s="1"/>
+      <c r="O93" s="26" t="e">
+        <f>SUM(M93:M94)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="15"/>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B94" s="22"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18">
+        <v>28</v>
+      </c>
+      <c r="E94" s="18"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I94" s="5"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N94" s="5"/>
+      <c r="O94" s="27"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="15"/>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B95" s="22"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18">
+        <v>29</v>
+      </c>
+      <c r="E95" s="18"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="15"/>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B96" s="22"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18">
+        <v>30</v>
+      </c>
+      <c r="E96" s="18"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3" t="e">
+        <f>AVERAGE(J96,K96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N96" s="3"/>
+      <c r="O96" s="10" t="e">
+        <f>M96</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1" t="e">
+        <f>O86/O96</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R96" s="15" t="e">
+        <f>1/Q96</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B97" s="22"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18">
+        <v>31</v>
+      </c>
+      <c r="E97" s="18"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1" t="e">
+        <f>AVERAGE(J97,K97)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N97" s="1"/>
+      <c r="O97" s="9" t="e">
+        <f t="shared" ref="O97:O100" si="26">M97</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1" t="e">
+        <f>O87/O97</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R97" s="15" t="e">
+        <f t="shared" ref="R97:R101" si="27">1/Q97</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="22"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18">
+        <v>33</v>
+      </c>
+      <c r="E98" s="18"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I98" s="1"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1" t="e">
+        <f>AVERAGE(J98,K98)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N98" s="1"/>
+      <c r="O98" s="9" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1" t="e">
+        <f>O88/O98</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R98" s="15" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B99" s="22"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18">
+        <v>36</v>
+      </c>
+      <c r="E99" s="18"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" s="1"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1" t="e">
+        <f>AVERAGE(J99,K99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N99" s="1"/>
+      <c r="O99" s="9" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1" t="e">
+        <f>O89/O99</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R99" s="15" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="22"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18">
+        <v>37</v>
+      </c>
+      <c r="E100" s="18"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" s="1"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1" t="e">
+        <f>AVERAGE(J100,K100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N100" s="1"/>
+      <c r="O100" s="9" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1" t="e">
+        <f>O91/O100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R100" s="15" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B101" s="22"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18">
+        <v>38</v>
+      </c>
+      <c r="E101" s="18"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="20"/>
+      <c r="H101" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I101" s="5"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="8" t="e">
+        <f t="shared" ref="M101" si="28">AVERAGE(J101,K101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N101" s="5"/>
+      <c r="O101" s="11" t="e">
+        <f>M101</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1" t="e">
+        <f>O93/O101</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R101" s="15" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B102" s="22"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18">
+        <v>43</v>
+      </c>
+      <c r="E102" s="18"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="15"/>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B103" s="22"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18">
+        <v>45</v>
+      </c>
+      <c r="E103" s="18"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="15"/>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B104" s="22"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18">
+        <v>47</v>
+      </c>
+      <c r="E104" s="18"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3">
+        <v>5.9300850000000001</v>
+      </c>
+      <c r="K104" s="3">
+        <v>6.0540060000000002</v>
+      </c>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3">
+        <f t="shared" ref="M104:M107" si="29">AVERAGE(J104,K104)</f>
+        <v>5.9920454999999997</v>
+      </c>
+      <c r="N104" s="3"/>
+      <c r="O104" s="10">
+        <f>M104</f>
+        <v>5.9920454999999997</v>
+      </c>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="15"/>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B105" s="22"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18">
+        <v>50</v>
+      </c>
+      <c r="E105" s="18"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I105" s="1"/>
+      <c r="J105" s="6">
+        <v>2.6552690000000001</v>
+      </c>
+      <c r="K105" s="6">
+        <v>2.7440199999999999</v>
+      </c>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1">
+        <f t="shared" si="29"/>
+        <v>2.6996444999999998</v>
+      </c>
+      <c r="N105" s="1"/>
+      <c r="O105" s="9">
+        <f t="shared" ref="O105:O106" si="30">M105</f>
+        <v>2.6996444999999998</v>
+      </c>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="15"/>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B106" s="22"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18">
+        <v>52</v>
+      </c>
+      <c r="E106" s="18"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="J106" s="6">
+        <v>5.3000000000000001E-5</v>
+      </c>
+      <c r="K106" s="6">
+        <v>5.44E-4</v>
+      </c>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1">
+        <f t="shared" si="29"/>
+        <v>2.9849999999999999E-4</v>
+      </c>
+      <c r="N106" s="1"/>
+      <c r="O106" s="9">
+        <f t="shared" si="30"/>
+        <v>2.9849999999999999E-4</v>
+      </c>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="15"/>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B107" s="22"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18">
+        <v>55</v>
+      </c>
+      <c r="E107" s="18"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I107" s="1"/>
+      <c r="J107" s="6">
+        <v>0.55580799999999997</v>
+      </c>
+      <c r="K107" s="6">
+        <v>0.58907900000000002</v>
+      </c>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1">
+        <f t="shared" si="29"/>
+        <v>0.57244349999999999</v>
+      </c>
+      <c r="N107" s="1"/>
+      <c r="O107" s="26">
+        <f>SUM(M107,M108,)</f>
+        <v>0.7543995</v>
+      </c>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="15"/>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B108" s="22"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18">
+        <v>56</v>
+      </c>
+      <c r="E108" s="18"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I108" s="1"/>
+      <c r="J108" s="6">
+        <v>0.17685400000000001</v>
+      </c>
+      <c r="K108" s="6">
+        <v>0.187058</v>
+      </c>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1">
+        <f>AVERAGE(J108,K108)</f>
+        <v>0.18195600000000001</v>
+      </c>
+      <c r="N108" s="1"/>
+      <c r="O108" s="26"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="15"/>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B109" s="22"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18">
+        <v>57</v>
+      </c>
+      <c r="E109" s="18"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I109" s="1"/>
+      <c r="J109" s="6">
+        <v>0.60735700000000004</v>
+      </c>
+      <c r="K109" s="6">
+        <v>0.64198500000000003</v>
+      </c>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1">
+        <f>AVERAGE(J109,K109)</f>
+        <v>0.62467099999999998</v>
+      </c>
+      <c r="N109" s="1"/>
+      <c r="O109" s="26">
+        <f>SUM(M109,M110)</f>
+        <v>0.82504650000000002</v>
+      </c>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="15"/>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B110" s="22"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18">
+        <v>61</v>
+      </c>
+      <c r="E110" s="18"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I110" s="1"/>
+      <c r="J110" s="6">
+        <v>0.19503100000000001</v>
+      </c>
+      <c r="K110" s="6">
+        <v>0.20571999999999999</v>
+      </c>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1">
+        <f t="shared" ref="M110:M112" si="31">AVERAGE(J110,K110)</f>
+        <v>0.20037549999999998</v>
+      </c>
+      <c r="N110" s="1"/>
+      <c r="O110" s="26"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="15"/>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B111" s="22"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18">
+        <v>64</v>
+      </c>
+      <c r="E111" s="18"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I111" s="1"/>
+      <c r="J111" s="6">
+        <v>0.44303100000000001</v>
+      </c>
+      <c r="K111" s="6">
+        <v>0.47302499999999997</v>
+      </c>
+      <c r="L111" s="1"/>
+      <c r="M111" s="6">
+        <f t="shared" si="31"/>
+        <v>0.45802799999999999</v>
+      </c>
+      <c r="N111" s="1"/>
+      <c r="O111" s="26">
+        <f>SUM(M111:M112)</f>
+        <v>0.60003849999999992</v>
+      </c>
+      <c r="P111" s="1"/>
+      <c r="Q111" s="1"/>
+      <c r="R111" s="15"/>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B112" s="22"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18">
+        <v>66</v>
+      </c>
+      <c r="E112" s="18"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I112" s="5"/>
+      <c r="J112" s="8">
+        <v>0.137491</v>
+      </c>
+      <c r="K112" s="8">
+        <v>0.14652999999999999</v>
+      </c>
+      <c r="L112" s="5"/>
+      <c r="M112" s="8">
+        <f t="shared" si="31"/>
+        <v>0.14201049999999998</v>
+      </c>
+      <c r="N112" s="5"/>
+      <c r="O112" s="27"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="15"/>
+    </row>
+    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B113" s="22"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18">
+        <v>70</v>
+      </c>
+      <c r="E113" s="18"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="15"/>
+    </row>
+    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B114" s="22"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18">
+        <v>71</v>
+      </c>
+      <c r="E114" s="18"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3">
+        <v>2.1222000000000001E-2</v>
+      </c>
+      <c r="K114" s="3">
+        <v>2.3970999999999999E-2</v>
+      </c>
+      <c r="L114" s="3"/>
+      <c r="M114" s="3">
+        <f>AVERAGE(J114,K114)</f>
+        <v>2.2596499999999999E-2</v>
+      </c>
+      <c r="N114" s="3"/>
+      <c r="O114" s="10">
+        <f>M114</f>
+        <v>2.2596499999999999E-2</v>
+      </c>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1">
+        <f>O104/O114</f>
+        <v>265.17582368950946</v>
+      </c>
+      <c r="R114" s="15">
+        <f>1/Q114</f>
+        <v>3.7710828464169702E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B115" s="22"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18">
+        <v>72</v>
+      </c>
+      <c r="E115" s="18"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I115" s="1"/>
+      <c r="J115" s="6">
+        <v>8.7840000000000001E-3</v>
+      </c>
+      <c r="K115" s="6">
+        <v>1.0426E-2</v>
+      </c>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1">
+        <f>AVERAGE(J115,K115)</f>
+        <v>9.604999999999999E-3</v>
+      </c>
+      <c r="N115" s="1"/>
+      <c r="O115" s="9">
+        <f t="shared" ref="O115:O118" si="32">M115</f>
+        <v>9.604999999999999E-3</v>
+      </c>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1">
+        <f>O105/O115</f>
+        <v>281.06657990629878</v>
+      </c>
+      <c r="R115" s="15">
+        <f t="shared" ref="R115:R119" si="33">1/Q115</f>
+        <v>3.5578758610624473E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B116" s="22"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18">
+        <v>73</v>
+      </c>
+      <c r="E116" s="18"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I116" s="1"/>
+      <c r="J116" s="6">
+        <v>1.8741000000000001E-2</v>
+      </c>
+      <c r="K116" s="6">
+        <v>2.5048999999999998E-2</v>
+      </c>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1">
+        <f>AVERAGE(J116,K116)</f>
+        <v>2.1894999999999998E-2</v>
+      </c>
+      <c r="N116" s="1"/>
+      <c r="O116" s="9">
+        <f t="shared" si="32"/>
+        <v>2.1894999999999998E-2</v>
+      </c>
+      <c r="P116" s="1"/>
+      <c r="Q116" s="1">
+        <f>O106/O116</f>
+        <v>1.3633249600365381E-2</v>
+      </c>
+      <c r="R116" s="15">
+        <f t="shared" si="33"/>
+        <v>73.350083752093795</v>
+      </c>
+    </row>
+    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B117" s="22"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18">
+        <v>75</v>
+      </c>
+      <c r="E117" s="18"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" s="1"/>
+      <c r="J117" s="6">
+        <v>5.4769999999999999E-2</v>
+      </c>
+      <c r="K117" s="6">
+        <v>5.6631000000000001E-2</v>
+      </c>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1">
+        <f>AVERAGE(J117,K117)</f>
+        <v>5.57005E-2</v>
+      </c>
+      <c r="N117" s="1"/>
+      <c r="O117" s="9">
+        <f t="shared" si="32"/>
+        <v>5.57005E-2</v>
+      </c>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="1">
+        <f>O107/O117</f>
+        <v>13.543855082090825</v>
+      </c>
+      <c r="R117" s="15">
+        <f t="shared" si="33"/>
+        <v>7.3834221788323023E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B118" s="22"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18">
+        <v>76</v>
+      </c>
+      <c r="E118" s="18"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="1"/>
+      <c r="J118" s="6">
+        <v>5.9110999999999997E-2</v>
+      </c>
+      <c r="K118" s="6">
+        <v>6.1005999999999998E-2</v>
+      </c>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1">
+        <f>AVERAGE(J118,K118)</f>
+        <v>6.0058500000000001E-2</v>
+      </c>
+      <c r="N118" s="1"/>
+      <c r="O118" s="9">
+        <f t="shared" si="32"/>
+        <v>6.0058500000000001E-2</v>
+      </c>
+      <c r="P118" s="1"/>
+      <c r="Q118" s="1">
+        <f>O109/O118</f>
+        <v>13.737381053472864</v>
+      </c>
+      <c r="R118" s="15">
+        <f t="shared" si="33"/>
+        <v>7.2794078879190441E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B119" s="22"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18">
+        <v>78</v>
+      </c>
+      <c r="E119" s="18"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I119" s="5"/>
+      <c r="J119" s="8">
+        <v>4.539E-2</v>
+      </c>
+      <c r="K119" s="8">
+        <v>4.7148000000000002E-2</v>
+      </c>
+      <c r="L119" s="5"/>
+      <c r="M119" s="8">
+        <f t="shared" ref="M119" si="34">AVERAGE(J119,K119)</f>
+        <v>4.6269000000000005E-2</v>
+      </c>
+      <c r="N119" s="5"/>
+      <c r="O119" s="11">
+        <f>M119</f>
+        <v>4.6269000000000005E-2</v>
+      </c>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="6">
+        <f>O111/O119</f>
+        <v>12.968477814519437</v>
+      </c>
+      <c r="R119" s="15">
+        <f t="shared" si="33"/>
+        <v>7.711005210498996E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B120" s="22"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="18">
+        <v>81</v>
+      </c>
+      <c r="E120" s="18"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+      <c r="Q120" s="1"/>
+      <c r="R120" s="15"/>
+    </row>
+    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B121" s="22"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="18">
+        <v>82</v>
+      </c>
+      <c r="E121" s="18"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+      <c r="P121" s="1"/>
+      <c r="Q121" s="1"/>
+      <c r="R121" s="15"/>
+    </row>
+    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B122" s="22"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18">
+        <v>83</v>
+      </c>
+      <c r="E122" s="18"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+      <c r="Q122" s="1"/>
+      <c r="R122" s="15"/>
+    </row>
+    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B123" s="22"/>
+      <c r="C123" s="18"/>
+      <c r="D123" s="18">
+        <v>86</v>
+      </c>
+      <c r="E123" s="18"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1"/>
+      <c r="P123" s="1"/>
+      <c r="Q123" s="1"/>
+      <c r="R123" s="15"/>
+    </row>
+    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B124" s="22"/>
+      <c r="C124" s="18"/>
+      <c r="D124" s="18">
+        <v>87</v>
+      </c>
+      <c r="E124" s="18"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+      <c r="Q124" s="1"/>
+      <c r="R124" s="15"/>
+    </row>
+    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B125" s="22"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="18">
+        <v>89</v>
+      </c>
+      <c r="E125" s="18"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1"/>
+      <c r="R125" s="15"/>
+    </row>
+    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B126" s="22"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="18">
+        <v>90</v>
+      </c>
+      <c r="E126" s="18"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="15"/>
+    </row>
+    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B127" s="22"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="18">
+        <v>98</v>
+      </c>
+      <c r="E127" s="18"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1"/>
+      <c r="P127" s="1"/>
+      <c r="Q127" s="1"/>
+      <c r="R127" s="15"/>
+    </row>
+    <row r="128" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B128" s="22"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="18">
+        <v>99</v>
+      </c>
+      <c r="E128" s="18"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="18"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+      <c r="N128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="P128" s="1"/>
+      <c r="Q128" s="1"/>
+      <c r="R128" s="15"/>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B129" s="22"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="18">
+        <v>100</v>
+      </c>
+      <c r="E129" s="18"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="18"/>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
+      <c r="O129" s="1"/>
+      <c r="P129" s="1"/>
+      <c r="Q129" s="1"/>
+      <c r="R129" s="15"/>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B130" s="22"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="18">
+        <v>103</v>
+      </c>
+      <c r="E130" s="18"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+      <c r="N130" s="1"/>
+      <c r="O130" s="1"/>
+      <c r="P130" s="1"/>
+      <c r="Q130" s="1"/>
+      <c r="R130" s="15"/>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B131" s="22"/>
+      <c r="C131" s="18"/>
+      <c r="D131" s="18">
+        <v>104</v>
+      </c>
+      <c r="E131" s="18"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+      <c r="O131" s="1"/>
+      <c r="P131" s="1"/>
+      <c r="Q131" s="1"/>
+      <c r="R131" s="15"/>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B132" s="22"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="18">
+        <v>107</v>
+      </c>
+      <c r="E132" s="18"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+      <c r="R132" s="15"/>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B133" s="22"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18">
+        <v>111</v>
+      </c>
+      <c r="E133" s="18"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+      <c r="Q133" s="1"/>
+      <c r="R133" s="15"/>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B134" s="22"/>
+      <c r="C134" s="18"/>
+      <c r="D134" s="18">
+        <v>112</v>
+      </c>
+      <c r="E134" s="18"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+      <c r="R134" s="15"/>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B135" s="22"/>
+      <c r="C135" s="18"/>
+      <c r="D135" s="18">
+        <v>113</v>
+      </c>
+      <c r="E135" s="18"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+      <c r="R135" s="15"/>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B136" s="22"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18">
+        <v>114</v>
+      </c>
+      <c r="E136" s="18"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+      <c r="N136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+      <c r="Q136" s="1"/>
+      <c r="R136" s="15"/>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B137" s="22"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18">
+        <v>116</v>
+      </c>
+      <c r="E137" s="18"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+      <c r="N137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
+      <c r="Q137" s="1"/>
+      <c r="R137" s="15"/>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B138" s="22"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18">
+        <v>118</v>
+      </c>
+      <c r="E138" s="18"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+      <c r="Q138" s="1"/>
+      <c r="R138" s="15"/>
+    </row>
+    <row r="139" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B139" s="22"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="18">
+        <v>119</v>
+      </c>
+      <c r="E139" s="18"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="15"/>
+    </row>
+    <row r="140" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B140" s="22"/>
+      <c r="C140" s="18"/>
+      <c r="D140" s="18">
+        <v>120</v>
+      </c>
+      <c r="E140" s="18"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="1"/>
+      <c r="R140" s="15"/>
+    </row>
+    <row r="141" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B141" s="22"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18">
+        <v>122</v>
+      </c>
+      <c r="E141" s="18"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
+      <c r="Q141" s="1"/>
+      <c r="R141" s="15"/>
+    </row>
+    <row r="142" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B142" s="22"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="18">
+        <v>124</v>
+      </c>
+      <c r="E142" s="18"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="15"/>
+    </row>
+    <row r="143" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="23"/>
+      <c r="C143" s="24"/>
+      <c r="D143" s="24"/>
+      <c r="E143" s="24"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="16"/>
+      <c r="I143" s="16"/>
+      <c r="J143" s="16"/>
+      <c r="K143" s="16"/>
+      <c r="L143" s="16"/>
+      <c r="M143" s="16"/>
+      <c r="N143" s="16"/>
+      <c r="O143" s="16"/>
+      <c r="P143" s="16"/>
+      <c r="Q143" s="16"/>
+      <c r="R143" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="O111:O112"/>
+    <mergeCell ref="O89:O90"/>
+    <mergeCell ref="O91:O92"/>
+    <mergeCell ref="O93:O94"/>
+    <mergeCell ref="O107:O108"/>
+    <mergeCell ref="O109:O110"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="O27:O28"/>

</xml_diff>

<commit_message>
Run with SA approach + results for liquid time = 5 days for all 1 vs 60
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="33">
   <si>
     <t>CVA</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Ratio Bilat / CCP</t>
+  </si>
+  <si>
+    <t>G2-G1</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S143"/>
+  <dimension ref="B1:S144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S116" sqref="S116"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +756,15 @@
       <c r="B4" s="22">
         <v>113</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="18">
         <v>0</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="19" t="s">
         <v>12</v>
@@ -3129,9 +3136,11 @@
         <v>27</v>
       </c>
       <c r="D84" s="18">
-        <v>3</v>
-      </c>
-      <c r="E84" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F84" s="1"/>
       <c r="G84" s="19" t="s">
         <v>29</v>
@@ -3152,9 +3161,11 @@
       <c r="B85" s="22"/>
       <c r="C85" s="18"/>
       <c r="D85" s="18">
-        <v>4</v>
-      </c>
-      <c r="E85" s="18"/>
+        <v>3</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -3173,9 +3184,11 @@
       <c r="B86" s="22"/>
       <c r="C86" s="18"/>
       <c r="D86" s="18">
-        <v>5</v>
-      </c>
-      <c r="E86" s="18"/>
+        <v>4</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F86" s="1"/>
       <c r="G86" s="2" t="s">
         <v>15</v>
@@ -3184,17 +3197,21 @@
         <v>0</v>
       </c>
       <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
+      <c r="J86" s="3">
+        <v>5.9226520000000002</v>
+      </c>
+      <c r="K86" s="3">
+        <v>6.0465109999999997</v>
+      </c>
       <c r="L86" s="3"/>
-      <c r="M86" s="3" t="e">
+      <c r="M86" s="3">
         <f t="shared" ref="M86:M89" si="23">AVERAGE(J86,K86)</f>
-        <v>#DIV/0!</v>
+        <v>5.9845815</v>
       </c>
       <c r="N86" s="3"/>
-      <c r="O86" s="10" t="e">
+      <c r="O86" s="10">
         <f>M86</f>
-        <v>#DIV/0!</v>
+        <v>5.9845815</v>
       </c>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
@@ -3204,26 +3221,32 @@
       <c r="B87" s="22"/>
       <c r="C87" s="18"/>
       <c r="D87" s="18">
-        <v>9</v>
-      </c>
-      <c r="E87" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F87" s="6"/>
       <c r="G87" s="4"/>
       <c r="H87" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
+      <c r="J87" s="1">
+        <v>2.6522540000000001</v>
+      </c>
+      <c r="K87" s="1">
+        <v>2.7410589999999999</v>
+      </c>
       <c r="L87" s="1"/>
-      <c r="M87" s="1" t="e">
+      <c r="M87" s="1">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
+        <v>2.6966565</v>
       </c>
       <c r="N87" s="1"/>
-      <c r="O87" s="9" t="e">
+      <c r="O87" s="9">
         <f t="shared" ref="O87:O88" si="24">M87</f>
-        <v>#DIV/0!</v>
+        <v>2.6966565</v>
       </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
@@ -3233,26 +3256,32 @@
       <c r="B88" s="22"/>
       <c r="C88" s="18"/>
       <c r="D88" s="18">
-        <v>13</v>
-      </c>
-      <c r="E88" s="25"/>
+        <v>9</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F88" s="6"/>
       <c r="G88" s="4"/>
       <c r="H88" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
+      <c r="J88" s="1">
+        <v>2.3499999999999999E-4</v>
+      </c>
+      <c r="K88" s="1">
+        <v>3.8200000000000002E-4</v>
+      </c>
       <c r="L88" s="1"/>
-      <c r="M88" s="1" t="e">
+      <c r="M88" s="1">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
+        <v>3.0850000000000002E-4</v>
       </c>
       <c r="N88" s="1"/>
-      <c r="O88" s="9" t="e">
+      <c r="O88" s="9">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>3.0850000000000002E-4</v>
       </c>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
@@ -3262,26 +3291,32 @@
       <c r="B89" s="22"/>
       <c r="C89" s="18"/>
       <c r="D89" s="18">
-        <v>17</v>
-      </c>
-      <c r="E89" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F89" s="6"/>
       <c r="G89" s="4"/>
       <c r="H89" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I89" s="1"/>
-      <c r="J89" s="6"/>
-      <c r="K89" s="6"/>
+      <c r="J89" s="6">
+        <v>0.63978699999999999</v>
+      </c>
+      <c r="K89" s="6">
+        <v>0.67512799999999995</v>
+      </c>
       <c r="L89" s="1"/>
-      <c r="M89" s="1" t="e">
+      <c r="M89" s="1">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
+        <v>0.65745750000000003</v>
       </c>
       <c r="N89" s="1"/>
-      <c r="O89" s="26" t="e">
+      <c r="O89" s="26">
         <f>SUM(M89,M90,)</f>
-        <v>#DIV/0!</v>
+        <v>0.86976000000000009</v>
       </c>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
@@ -3291,21 +3326,27 @@
       <c r="B90" s="22"/>
       <c r="C90" s="18"/>
       <c r="D90" s="18">
-        <v>24</v>
-      </c>
-      <c r="E90" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="E90" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F90" s="6"/>
       <c r="G90" s="4"/>
       <c r="H90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I90" s="1"/>
-      <c r="J90" s="6"/>
-      <c r="K90" s="6"/>
+      <c r="J90" s="6">
+        <v>0.20680999999999999</v>
+      </c>
+      <c r="K90" s="6">
+        <v>0.21779499999999999</v>
+      </c>
       <c r="L90" s="1"/>
-      <c r="M90" s="1" t="e">
+      <c r="M90" s="1">
         <f>AVERAGE(J90,K90)</f>
-        <v>#DIV/0!</v>
+        <v>0.21230250000000001</v>
       </c>
       <c r="N90" s="1"/>
       <c r="O90" s="26"/>
@@ -3317,26 +3358,32 @@
       <c r="B91" s="22"/>
       <c r="C91" s="18"/>
       <c r="D91" s="18">
-        <v>25</v>
-      </c>
-      <c r="E91" s="25"/>
+        <v>24</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F91" s="6"/>
       <c r="G91" s="4"/>
       <c r="H91" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I91" s="1"/>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
+      <c r="J91" s="6">
+        <v>0.74666900000000003</v>
+      </c>
+      <c r="K91" s="6">
+        <v>0.78458000000000006</v>
+      </c>
       <c r="L91" s="1"/>
-      <c r="M91" s="1" t="e">
+      <c r="M91" s="1">
         <f>AVERAGE(J91,K91)</f>
-        <v>#DIV/0!</v>
+        <v>0.76562450000000004</v>
       </c>
       <c r="N91" s="1"/>
-      <c r="O91" s="26" t="e">
+      <c r="O91" s="26">
         <f>SUM(M91,M92)</f>
-        <v>#DIV/0!</v>
+        <v>1.0163905</v>
       </c>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
@@ -3346,21 +3393,27 @@
       <c r="B92" s="22"/>
       <c r="C92" s="18"/>
       <c r="D92" s="18">
-        <v>26</v>
-      </c>
-      <c r="E92" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F92" s="6"/>
       <c r="G92" s="4"/>
       <c r="H92" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I92" s="1"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
+      <c r="J92" s="6">
+        <v>0.24480399999999999</v>
+      </c>
+      <c r="K92" s="6">
+        <v>0.25672800000000001</v>
+      </c>
       <c r="L92" s="1"/>
-      <c r="M92" s="1" t="e">
+      <c r="M92" s="1">
         <f t="shared" ref="M92:M94" si="25">AVERAGE(J92,K92)</f>
-        <v>#DIV/0!</v>
+        <v>0.25076599999999999</v>
       </c>
       <c r="N92" s="1"/>
       <c r="O92" s="26"/>
@@ -3372,26 +3425,32 @@
       <c r="B93" s="22"/>
       <c r="C93" s="18"/>
       <c r="D93" s="18">
-        <v>27</v>
-      </c>
-      <c r="E93" s="25"/>
+        <v>26</v>
+      </c>
+      <c r="E93" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="F93" s="6"/>
       <c r="G93" s="4"/>
       <c r="H93" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I93" s="1"/>
-      <c r="J93" s="6"/>
-      <c r="K93" s="6"/>
+      <c r="J93" s="6">
+        <v>0.42064699999999999</v>
+      </c>
+      <c r="K93" s="6">
+        <v>0.44994499999999998</v>
+      </c>
       <c r="L93" s="1"/>
-      <c r="M93" s="6" t="e">
+      <c r="M93" s="6">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.43529600000000002</v>
       </c>
       <c r="N93" s="1"/>
-      <c r="O93" s="26" t="e">
+      <c r="O93" s="26">
         <f>SUM(M93:M94)</f>
-        <v>#DIV/0!</v>
+        <v>0.56950100000000003</v>
       </c>
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
@@ -3401,21 +3460,27 @@
       <c r="B94" s="22"/>
       <c r="C94" s="18"/>
       <c r="D94" s="18">
-        <v>28</v>
-      </c>
-      <c r="E94" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F94" s="1"/>
       <c r="G94" s="20"/>
       <c r="H94" s="8" t="s">
         <v>20</v>
       </c>
       <c r="I94" s="5"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
+      <c r="J94" s="8">
+        <v>0.12981000000000001</v>
+      </c>
+      <c r="K94" s="8">
+        <v>0.1386</v>
+      </c>
       <c r="L94" s="5"/>
-      <c r="M94" s="8" t="e">
+      <c r="M94" s="8">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0.13420500000000002</v>
       </c>
       <c r="N94" s="5"/>
       <c r="O94" s="27"/>
@@ -3427,9 +3492,11 @@
       <c r="B95" s="22"/>
       <c r="C95" s="18"/>
       <c r="D95" s="18">
-        <v>29</v>
-      </c>
-      <c r="E95" s="18"/>
+        <v>28</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -3448,9 +3515,11 @@
       <c r="B96" s="22"/>
       <c r="C96" s="18"/>
       <c r="D96" s="18">
-        <v>30</v>
-      </c>
-      <c r="E96" s="18"/>
+        <v>29</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F96" s="1"/>
       <c r="G96" s="2" t="s">
         <v>13</v>
@@ -3459,210 +3528,246 @@
         <v>0</v>
       </c>
       <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
+      <c r="J96" s="3">
+        <v>2.9817E-2</v>
+      </c>
+      <c r="K96" s="3">
+        <v>3.3932999999999998E-2</v>
+      </c>
       <c r="L96" s="3"/>
-      <c r="M96" s="3" t="e">
+      <c r="M96" s="3">
         <f>AVERAGE(J96,K96)</f>
-        <v>#DIV/0!</v>
+        <v>3.1875000000000001E-2</v>
       </c>
       <c r="N96" s="3"/>
-      <c r="O96" s="10" t="e">
+      <c r="O96" s="10">
         <f>M96</f>
-        <v>#DIV/0!</v>
+        <v>3.1875000000000001E-2</v>
       </c>
       <c r="P96" s="1"/>
-      <c r="Q96" s="1" t="e">
+      <c r="Q96" s="1">
         <f>O86/O96</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R96" s="15" t="e">
+        <v>187.75157647058822</v>
+      </c>
+      <c r="R96" s="15">
         <f>1/Q96</f>
-        <v>#DIV/0!</v>
+        <v>5.3261869689634946E-3</v>
       </c>
     </row>
     <row r="97" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B97" s="22"/>
       <c r="C97" s="18"/>
       <c r="D97" s="18">
-        <v>31</v>
-      </c>
-      <c r="E97" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F97" s="1"/>
       <c r="G97" s="4"/>
       <c r="H97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I97" s="1"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="6"/>
+      <c r="J97" s="6">
+        <v>1.8998999999999999E-2</v>
+      </c>
+      <c r="K97" s="6">
+        <v>2.2457000000000001E-2</v>
+      </c>
       <c r="L97" s="1"/>
-      <c r="M97" s="1" t="e">
+      <c r="M97" s="1">
         <f>AVERAGE(J97,K97)</f>
-        <v>#DIV/0!</v>
+        <v>2.0728E-2</v>
       </c>
       <c r="N97" s="1"/>
-      <c r="O97" s="9" t="e">
+      <c r="O97" s="9">
         <f t="shared" ref="O97:O100" si="26">M97</f>
-        <v>#DIV/0!</v>
+        <v>2.0728E-2</v>
       </c>
       <c r="P97" s="1"/>
-      <c r="Q97" s="1" t="e">
+      <c r="Q97" s="1">
         <f>O87/O97</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R97" s="15" t="e">
+        <v>130.09728386723273</v>
+      </c>
+      <c r="R97" s="15">
         <f t="shared" ref="R97:R101" si="27">1/Q97</f>
-        <v>#DIV/0!</v>
+        <v>7.6865555549993107E-3</v>
       </c>
     </row>
     <row r="98" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B98" s="22"/>
       <c r="C98" s="18"/>
       <c r="D98" s="18">
-        <v>33</v>
-      </c>
-      <c r="E98" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F98" s="1"/>
       <c r="G98" s="4"/>
       <c r="H98" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I98" s="1"/>
-      <c r="J98" s="6"/>
-      <c r="K98" s="6"/>
+      <c r="J98" s="6">
+        <v>3.3314999999999997E-2</v>
+      </c>
+      <c r="K98" s="6">
+        <v>3.9480000000000001E-2</v>
+      </c>
       <c r="L98" s="1"/>
-      <c r="M98" s="1" t="e">
+      <c r="M98" s="1">
         <f>AVERAGE(J98,K98)</f>
-        <v>#DIV/0!</v>
+        <v>3.6397499999999999E-2</v>
       </c>
       <c r="N98" s="1"/>
-      <c r="O98" s="9" t="e">
+      <c r="O98" s="9">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>3.6397499999999999E-2</v>
       </c>
       <c r="P98" s="1"/>
-      <c r="Q98" s="1" t="e">
+      <c r="Q98" s="1">
         <f>O88/O98</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R98" s="15" t="e">
+        <v>8.4758568583007086E-3</v>
+      </c>
+      <c r="R98" s="15">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>117.98217179902754</v>
       </c>
     </row>
     <row r="99" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B99" s="22"/>
       <c r="C99" s="18"/>
       <c r="D99" s="18">
-        <v>36</v>
-      </c>
-      <c r="E99" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F99" s="1"/>
       <c r="G99" s="4"/>
       <c r="H99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I99" s="1"/>
-      <c r="J99" s="6"/>
-      <c r="K99" s="6"/>
+      <c r="J99" s="6">
+        <v>6.0169E-2</v>
+      </c>
+      <c r="K99" s="6">
+        <v>6.2130999999999999E-2</v>
+      </c>
       <c r="L99" s="1"/>
-      <c r="M99" s="1" t="e">
+      <c r="M99" s="1">
         <f>AVERAGE(J99,K99)</f>
-        <v>#DIV/0!</v>
+        <v>6.1149999999999996E-2</v>
       </c>
       <c r="N99" s="1"/>
-      <c r="O99" s="9" t="e">
+      <c r="O99" s="9">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>6.1149999999999996E-2</v>
       </c>
       <c r="P99" s="1"/>
-      <c r="Q99" s="1" t="e">
+      <c r="Q99" s="1">
         <f>O89/O99</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R99" s="15" t="e">
+        <v>14.223385118560918</v>
+      </c>
+      <c r="R99" s="15">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>7.0306751287711536E-2</v>
       </c>
     </row>
     <row r="100" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B100" s="22"/>
       <c r="C100" s="18"/>
       <c r="D100" s="18">
-        <v>37</v>
-      </c>
-      <c r="E100" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F100" s="1"/>
       <c r="G100" s="4"/>
       <c r="H100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I100" s="1"/>
-      <c r="J100" s="6"/>
-      <c r="K100" s="6"/>
+      <c r="J100" s="6">
+        <v>6.8520999999999999E-2</v>
+      </c>
+      <c r="K100" s="6">
+        <v>7.0539000000000004E-2</v>
+      </c>
       <c r="L100" s="1"/>
-      <c r="M100" s="1" t="e">
+      <c r="M100" s="1">
         <f>AVERAGE(J100,K100)</f>
-        <v>#DIV/0!</v>
+        <v>6.9530000000000008E-2</v>
       </c>
       <c r="N100" s="1"/>
-      <c r="O100" s="9" t="e">
+      <c r="O100" s="9">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>6.9530000000000008E-2</v>
       </c>
       <c r="P100" s="1"/>
-      <c r="Q100" s="1" t="e">
+      <c r="Q100" s="1">
         <f>O91/O100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R100" s="15" t="e">
+        <v>14.618013806989786</v>
+      </c>
+      <c r="R100" s="15">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>6.8408746441451396E-2</v>
       </c>
     </row>
     <row r="101" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B101" s="22"/>
       <c r="C101" s="18"/>
       <c r="D101" s="18">
-        <v>38</v>
-      </c>
-      <c r="E101" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F101" s="1"/>
       <c r="G101" s="20"/>
       <c r="H101" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I101" s="5"/>
-      <c r="J101" s="8"/>
-      <c r="K101" s="8"/>
+      <c r="J101" s="8">
+        <v>4.3298999999999997E-2</v>
+      </c>
+      <c r="K101" s="8">
+        <v>4.5069999999999999E-2</v>
+      </c>
       <c r="L101" s="5"/>
-      <c r="M101" s="8" t="e">
+      <c r="M101" s="8">
         <f t="shared" ref="M101" si="28">AVERAGE(J101,K101)</f>
-        <v>#DIV/0!</v>
+        <v>4.4184500000000002E-2</v>
       </c>
       <c r="N101" s="5"/>
-      <c r="O101" s="11" t="e">
+      <c r="O101" s="11">
         <f>M101</f>
-        <v>#DIV/0!</v>
+        <v>4.4184500000000002E-2</v>
       </c>
       <c r="P101" s="1"/>
-      <c r="Q101" s="1" t="e">
+      <c r="Q101" s="1">
         <f>O93/O101</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R101" s="15" t="e">
+        <v>12.889157962633956</v>
+      </c>
+      <c r="R101" s="15">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>7.7584587208802083E-2</v>
       </c>
     </row>
     <row r="102" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B102" s="22"/>
       <c r="C102" s="18"/>
       <c r="D102" s="18">
-        <v>43</v>
-      </c>
-      <c r="E102" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="E102" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
@@ -3681,9 +3786,11 @@
       <c r="B103" s="22"/>
       <c r="C103" s="18"/>
       <c r="D103" s="18">
-        <v>45</v>
-      </c>
-      <c r="E103" s="18"/>
+        <v>43</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
@@ -3702,9 +3809,11 @@
       <c r="B104" s="22"/>
       <c r="C104" s="18"/>
       <c r="D104" s="18">
-        <v>47</v>
-      </c>
-      <c r="E104" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F104" s="1"/>
       <c r="G104" s="2" t="s">
         <v>16</v>
@@ -3737,9 +3846,11 @@
       <c r="B105" s="22"/>
       <c r="C105" s="18"/>
       <c r="D105" s="18">
-        <v>50</v>
-      </c>
-      <c r="E105" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F105" s="1"/>
       <c r="G105" s="4"/>
       <c r="H105" s="1" t="s">
@@ -3770,9 +3881,11 @@
       <c r="B106" s="22"/>
       <c r="C106" s="18"/>
       <c r="D106" s="18">
-        <v>52</v>
-      </c>
-      <c r="E106" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="E106" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F106" s="1"/>
       <c r="G106" s="4"/>
       <c r="H106" s="1" t="s">
@@ -3803,9 +3916,11 @@
       <c r="B107" s="22"/>
       <c r="C107" s="18"/>
       <c r="D107" s="18">
-        <v>55</v>
-      </c>
-      <c r="E107" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F107" s="1"/>
       <c r="G107" s="4"/>
       <c r="H107" s="1" t="s">
@@ -3836,9 +3951,11 @@
       <c r="B108" s="22"/>
       <c r="C108" s="18"/>
       <c r="D108" s="18">
-        <v>56</v>
-      </c>
-      <c r="E108" s="18"/>
+        <v>55</v>
+      </c>
+      <c r="E108" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F108" s="1"/>
       <c r="G108" s="4"/>
       <c r="H108" s="1" t="s">
@@ -3866,9 +3983,11 @@
       <c r="B109" s="22"/>
       <c r="C109" s="18"/>
       <c r="D109" s="18">
-        <v>57</v>
-      </c>
-      <c r="E109" s="18"/>
+        <v>56</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F109" s="1"/>
       <c r="G109" s="4"/>
       <c r="H109" s="1" t="s">
@@ -3899,9 +4018,11 @@
       <c r="B110" s="22"/>
       <c r="C110" s="18"/>
       <c r="D110" s="18">
-        <v>61</v>
-      </c>
-      <c r="E110" s="18"/>
+        <v>57</v>
+      </c>
+      <c r="E110" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F110" s="1"/>
       <c r="G110" s="4"/>
       <c r="H110" s="1" t="s">
@@ -3929,9 +4050,11 @@
       <c r="B111" s="22"/>
       <c r="C111" s="18"/>
       <c r="D111" s="18">
-        <v>64</v>
-      </c>
-      <c r="E111" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F111" s="1"/>
       <c r="G111" s="4"/>
       <c r="H111" s="6" t="s">
@@ -3962,9 +4085,11 @@
       <c r="B112" s="22"/>
       <c r="C112" s="18"/>
       <c r="D112" s="18">
-        <v>66</v>
-      </c>
-      <c r="E112" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F112" s="1"/>
       <c r="G112" s="20"/>
       <c r="H112" s="8" t="s">
@@ -3992,9 +4117,11 @@
       <c r="B113" s="22"/>
       <c r="C113" s="18"/>
       <c r="D113" s="18">
-        <v>70</v>
-      </c>
-      <c r="E113" s="18"/>
+        <v>66</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
@@ -4013,9 +4140,11 @@
       <c r="B114" s="22"/>
       <c r="C114" s="18"/>
       <c r="D114" s="18">
-        <v>71</v>
-      </c>
-      <c r="E114" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="E114" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F114" s="1"/>
       <c r="G114" s="2" t="s">
         <v>14</v>
@@ -4054,9 +4183,11 @@
       <c r="B115" s="22"/>
       <c r="C115" s="18"/>
       <c r="D115" s="18">
-        <v>72</v>
-      </c>
-      <c r="E115" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F115" s="1"/>
       <c r="G115" s="4"/>
       <c r="H115" s="1" t="s">
@@ -4093,9 +4224,11 @@
       <c r="B116" s="22"/>
       <c r="C116" s="18"/>
       <c r="D116" s="18">
-        <v>73</v>
-      </c>
-      <c r="E116" s="18"/>
+        <v>72</v>
+      </c>
+      <c r="E116" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F116" s="1"/>
       <c r="G116" s="4"/>
       <c r="H116" s="1" t="s">
@@ -4132,9 +4265,11 @@
       <c r="B117" s="22"/>
       <c r="C117" s="18"/>
       <c r="D117" s="18">
-        <v>75</v>
-      </c>
-      <c r="E117" s="18"/>
+        <v>73</v>
+      </c>
+      <c r="E117" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F117" s="1"/>
       <c r="G117" s="4"/>
       <c r="H117" s="1" t="s">
@@ -4171,9 +4306,11 @@
       <c r="B118" s="22"/>
       <c r="C118" s="18"/>
       <c r="D118" s="18">
-        <v>76</v>
-      </c>
-      <c r="E118" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="E118" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="F118" s="1"/>
       <c r="G118" s="4"/>
       <c r="H118" s="1" t="s">
@@ -4210,9 +4347,11 @@
       <c r="B119" s="22"/>
       <c r="C119" s="18"/>
       <c r="D119" s="18">
-        <v>78</v>
-      </c>
-      <c r="E119" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="E119" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F119" s="1"/>
       <c r="G119" s="20"/>
       <c r="H119" s="8" t="s">
@@ -4249,9 +4388,11 @@
       <c r="B120" s="22"/>
       <c r="C120" s="18"/>
       <c r="D120" s="18">
-        <v>81</v>
-      </c>
-      <c r="E120" s="18"/>
+        <v>78</v>
+      </c>
+      <c r="E120" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -4270,9 +4411,11 @@
       <c r="B121" s="22"/>
       <c r="C121" s="18"/>
       <c r="D121" s="18">
-        <v>82</v>
-      </c>
-      <c r="E121" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="E121" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -4291,9 +4434,11 @@
       <c r="B122" s="22"/>
       <c r="C122" s="18"/>
       <c r="D122" s="18">
-        <v>83</v>
-      </c>
-      <c r="E122" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="E122" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -4312,9 +4457,11 @@
       <c r="B123" s="22"/>
       <c r="C123" s="18"/>
       <c r="D123" s="18">
-        <v>86</v>
-      </c>
-      <c r="E123" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="E123" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -4333,9 +4480,11 @@
       <c r="B124" s="22"/>
       <c r="C124" s="18"/>
       <c r="D124" s="18">
-        <v>87</v>
-      </c>
-      <c r="E124" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="E124" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -4354,9 +4503,11 @@
       <c r="B125" s="22"/>
       <c r="C125" s="18"/>
       <c r="D125" s="18">
-        <v>89</v>
-      </c>
-      <c r="E125" s="18"/>
+        <v>87</v>
+      </c>
+      <c r="E125" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -4375,9 +4526,11 @@
       <c r="B126" s="22"/>
       <c r="C126" s="28"/>
       <c r="D126" s="18">
-        <v>90</v>
-      </c>
-      <c r="E126" s="18"/>
+        <v>89</v>
+      </c>
+      <c r="E126" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -4396,9 +4549,11 @@
       <c r="B127" s="22"/>
       <c r="C127" s="18"/>
       <c r="D127" s="18">
-        <v>98</v>
-      </c>
-      <c r="E127" s="18"/>
+        <v>90</v>
+      </c>
+      <c r="E127" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -4417,9 +4572,11 @@
       <c r="B128" s="22"/>
       <c r="C128" s="18"/>
       <c r="D128" s="18">
-        <v>99</v>
-      </c>
-      <c r="E128" s="18"/>
+        <v>98</v>
+      </c>
+      <c r="E128" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="18"/>
@@ -4438,9 +4595,11 @@
       <c r="B129" s="22"/>
       <c r="C129" s="18"/>
       <c r="D129" s="18">
-        <v>100</v>
-      </c>
-      <c r="E129" s="18"/>
+        <v>99</v>
+      </c>
+      <c r="E129" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="18"/>
@@ -4459,9 +4618,11 @@
       <c r="B130" s="22"/>
       <c r="C130" s="18"/>
       <c r="D130" s="18">
-        <v>103</v>
-      </c>
-      <c r="E130" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="E130" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
@@ -4480,9 +4641,11 @@
       <c r="B131" s="22"/>
       <c r="C131" s="18"/>
       <c r="D131" s="18">
-        <v>104</v>
-      </c>
-      <c r="E131" s="18"/>
+        <v>103</v>
+      </c>
+      <c r="E131" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -4501,9 +4664,11 @@
       <c r="B132" s="22"/>
       <c r="C132" s="18"/>
       <c r="D132" s="18">
-        <v>107</v>
-      </c>
-      <c r="E132" s="18"/>
+        <v>104</v>
+      </c>
+      <c r="E132" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -4522,9 +4687,11 @@
       <c r="B133" s="22"/>
       <c r="C133" s="18"/>
       <c r="D133" s="18">
-        <v>111</v>
-      </c>
-      <c r="E133" s="18"/>
+        <v>107</v>
+      </c>
+      <c r="E133" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -4543,9 +4710,11 @@
       <c r="B134" s="22"/>
       <c r="C134" s="18"/>
       <c r="D134" s="18">
-        <v>112</v>
-      </c>
-      <c r="E134" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="E134" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -4564,9 +4733,11 @@
       <c r="B135" s="22"/>
       <c r="C135" s="18"/>
       <c r="D135" s="18">
-        <v>113</v>
-      </c>
-      <c r="E135" s="18"/>
+        <v>112</v>
+      </c>
+      <c r="E135" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
@@ -4585,9 +4756,11 @@
       <c r="B136" s="22"/>
       <c r="C136" s="18"/>
       <c r="D136" s="18">
-        <v>114</v>
-      </c>
-      <c r="E136" s="18"/>
+        <v>113</v>
+      </c>
+      <c r="E136" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -4606,9 +4779,11 @@
       <c r="B137" s="22"/>
       <c r="C137" s="18"/>
       <c r="D137" s="18">
-        <v>116</v>
-      </c>
-      <c r="E137" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="E137" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -4627,9 +4802,11 @@
       <c r="B138" s="22"/>
       <c r="C138" s="18"/>
       <c r="D138" s="18">
-        <v>118</v>
-      </c>
-      <c r="E138" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="E138" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -4648,9 +4825,11 @@
       <c r="B139" s="22"/>
       <c r="C139" s="18"/>
       <c r="D139" s="18">
-        <v>119</v>
-      </c>
-      <c r="E139" s="18"/>
+        <v>118</v>
+      </c>
+      <c r="E139" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
@@ -4669,9 +4848,11 @@
       <c r="B140" s="22"/>
       <c r="C140" s="18"/>
       <c r="D140" s="18">
-        <v>120</v>
-      </c>
-      <c r="E140" s="18"/>
+        <v>119</v>
+      </c>
+      <c r="E140" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
@@ -4690,9 +4871,11 @@
       <c r="B141" s="22"/>
       <c r="C141" s="18"/>
       <c r="D141" s="18">
-        <v>122</v>
-      </c>
-      <c r="E141" s="18"/>
+        <v>120</v>
+      </c>
+      <c r="E141" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
@@ -4711,9 +4894,11 @@
       <c r="B142" s="22"/>
       <c r="C142" s="18"/>
       <c r="D142" s="18">
-        <v>124</v>
-      </c>
-      <c r="E142" s="18"/>
+        <v>122</v>
+      </c>
+      <c r="E142" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
@@ -4728,24 +4913,47 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="15"/>
     </row>
-    <row r="143" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="23"/>
-      <c r="C143" s="24"/>
-      <c r="D143" s="24"/>
-      <c r="E143" s="24"/>
-      <c r="F143" s="16"/>
-      <c r="G143" s="16"/>
-      <c r="H143" s="16"/>
-      <c r="I143" s="16"/>
-      <c r="J143" s="16"/>
-      <c r="K143" s="16"/>
-      <c r="L143" s="16"/>
-      <c r="M143" s="16"/>
-      <c r="N143" s="16"/>
-      <c r="O143" s="16"/>
-      <c r="P143" s="16"/>
-      <c r="Q143" s="16"/>
-      <c r="R143" s="17"/>
+    <row r="143" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B143" s="22"/>
+      <c r="C143" s="18"/>
+      <c r="D143" s="18">
+        <v>124</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="15"/>
+    </row>
+    <row r="144" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="23"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="16"/>
+      <c r="I144" s="16"/>
+      <c r="J144" s="16"/>
+      <c r="K144" s="16"/>
+      <c r="L144" s="16"/>
+      <c r="M144" s="16"/>
+      <c r="N144" s="16"/>
+      <c r="O144" s="16"/>
+      <c r="P144" s="16"/>
+      <c r="Q144" s="16"/>
+      <c r="R144" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
New run for 60 vs 1, old was incorrect
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -367,14 +367,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>0.45610399999999995</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="26">
+      <c r="O9" s="27">
         <f>SUM(M9,M10,)</f>
         <v>0.61037849999999993</v>
       </c>
@@ -949,7 +949,7 @@
         <v>0.15427450000000001</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="26"/>
+      <c r="O10" s="27"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="15"/>
@@ -977,7 +977,7 @@
         <v>0.53189200000000003</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="26">
+      <c r="O11" s="27">
         <f>SUM(M11,M12)</f>
         <v>0.7136975000000001</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>0.18180550000000001</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="26"/>
+      <c r="O12" s="27"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="15"/>
@@ -1036,7 +1036,7 @@
         <v>0.30064199999999996</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="26">
+      <c r="O13" s="27">
         <f>SUM(M13:M14)</f>
         <v>0.39890049999999999</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>9.8258499999999999E-2</v>
       </c>
       <c r="N14" s="5"/>
-      <c r="O14" s="27"/>
+      <c r="O14" s="28"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="15"/>
@@ -1471,7 +1471,7 @@
         <v>0.39651199999999998</v>
       </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="26">
+      <c r="O27" s="27">
         <f>SUM(M27,M28,)</f>
         <v>0.52906750000000002</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>0.13255549999999999</v>
       </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="26"/>
+      <c r="O28" s="27"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="15"/>
@@ -1530,7 +1530,7 @@
         <v>0.43305550000000004</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="26">
+      <c r="O29" s="27">
         <f>SUM(M29,M30)</f>
         <v>0.57880550000000008</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0.14574999999999999</v>
       </c>
       <c r="N30" s="1"/>
-      <c r="O30" s="26"/>
+      <c r="O30" s="27"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="15"/>
@@ -1589,7 +1589,7 @@
         <v>0.31654399999999999</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="26">
+      <c r="O31" s="27">
         <f>SUM(M31:M32)</f>
         <v>0.420427</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0.103883</v>
       </c>
       <c r="N32" s="5"/>
-      <c r="O32" s="27"/>
+      <c r="O32" s="28"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="15"/>
@@ -2123,7 +2123,7 @@
         <v>0.57179449999999998</v>
       </c>
       <c r="N49" s="1"/>
-      <c r="O49" s="26">
+      <c r="O49" s="27">
         <f>SUM(M49,M50,)</f>
         <v>1.2137245000000001</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.64193</v>
       </c>
       <c r="N50" s="1"/>
-      <c r="O50" s="26"/>
+      <c r="O50" s="27"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="15"/>
@@ -2190,7 +2190,7 @@
         <v>0.66603649999999992</v>
       </c>
       <c r="N51" s="1"/>
-      <c r="O51" s="26">
+      <c r="O51" s="27">
         <f>SUM(M51,M52)</f>
         <v>1.4226604999999999</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0.75662399999999996</v>
       </c>
       <c r="N52" s="1"/>
-      <c r="O52" s="26"/>
+      <c r="O52" s="27"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="15"/>
@@ -2257,7 +2257,7 @@
         <v>0.37829049999999997</v>
       </c>
       <c r="N53" s="1"/>
-      <c r="O53" s="26">
+      <c r="O53" s="27">
         <f>SUM(M53:M54)</f>
         <v>0.78686499999999993</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0.40857450000000001</v>
       </c>
       <c r="N54" s="5"/>
-      <c r="O54" s="27"/>
+      <c r="O54" s="28"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="15"/>
@@ -2692,7 +2692,7 @@
         <v>0.4977125</v>
       </c>
       <c r="N67" s="1"/>
-      <c r="O67" s="26">
+      <c r="O67" s="27">
         <f>SUM(M67,M68,)</f>
         <v>1.0491809999999999</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0.55146849999999992</v>
       </c>
       <c r="N68" s="1"/>
-      <c r="O68" s="26"/>
+      <c r="O68" s="27"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="15"/>
@@ -2751,7 +2751,7 @@
         <v>0.54320349999999995</v>
       </c>
       <c r="N69" s="1"/>
-      <c r="O69" s="26">
+      <c r="O69" s="27">
         <f>SUM(M69,M70)</f>
         <v>1.1496564999999999</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>0.60645300000000002</v>
       </c>
       <c r="N70" s="1"/>
-      <c r="O70" s="26"/>
+      <c r="O70" s="27"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="15"/>
@@ -2810,7 +2810,7 @@
         <v>0.39807099999999995</v>
       </c>
       <c r="N71" s="1"/>
-      <c r="O71" s="26">
+      <c r="O71" s="27">
         <f>SUM(M71:M72)</f>
         <v>0.83006349999999995</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>0.4319925</v>
       </c>
       <c r="N72" s="5"/>
-      <c r="O72" s="27"/>
+      <c r="O72" s="28"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="15"/>
@@ -3314,7 +3314,7 @@
         <v>0.65745750000000003</v>
       </c>
       <c r="N89" s="1"/>
-      <c r="O89" s="26">
+      <c r="O89" s="27">
         <f>SUM(M89,M90,)</f>
         <v>0.86976000000000009</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>0.21230250000000001</v>
       </c>
       <c r="N90" s="1"/>
-      <c r="O90" s="26"/>
+      <c r="O90" s="27"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="15"/>
@@ -3381,7 +3381,7 @@
         <v>0.76562450000000004</v>
       </c>
       <c r="N91" s="1"/>
-      <c r="O91" s="26">
+      <c r="O91" s="27">
         <f>SUM(M91,M92)</f>
         <v>1.0163905</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>0.25076599999999999</v>
       </c>
       <c r="N92" s="1"/>
-      <c r="O92" s="26"/>
+      <c r="O92" s="27"/>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
       <c r="R92" s="15"/>
@@ -3448,7 +3448,7 @@
         <v>0.43529600000000002</v>
       </c>
       <c r="N93" s="1"/>
-      <c r="O93" s="26">
+      <c r="O93" s="27">
         <f>SUM(M93:M94)</f>
         <v>0.56950100000000003</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>0.13420500000000002</v>
       </c>
       <c r="N94" s="5"/>
-      <c r="O94" s="27"/>
+      <c r="O94" s="28"/>
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
       <c r="R94" s="15"/>
@@ -3529,29 +3529,29 @@
       </c>
       <c r="I96" s="3"/>
       <c r="J96" s="3">
-        <v>2.9817E-2</v>
+        <v>1.9758999999999999E-2</v>
       </c>
       <c r="K96" s="3">
-        <v>3.3932999999999998E-2</v>
+        <v>2.1950000000000001E-2</v>
       </c>
       <c r="L96" s="3"/>
       <c r="M96" s="3">
         <f>AVERAGE(J96,K96)</f>
-        <v>3.1875000000000001E-2</v>
+        <v>2.0854499999999998E-2</v>
       </c>
       <c r="N96" s="3"/>
       <c r="O96" s="10">
         <f>M96</f>
-        <v>3.1875000000000001E-2</v>
+        <v>2.0854499999999998E-2</v>
       </c>
       <c r="P96" s="1"/>
       <c r="Q96" s="1">
         <f>O86/O96</f>
-        <v>187.75157647058822</v>
+        <v>286.96835215421135</v>
       </c>
       <c r="R96" s="15">
         <f>1/Q96</f>
-        <v>5.3261869689634946E-3</v>
+        <v>3.4847048202117387E-3</v>
       </c>
     </row>
     <row r="97" spans="2:18" x14ac:dyDescent="0.25">
@@ -3652,29 +3652,29 @@
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="6">
-        <v>6.0169E-2</v>
+        <v>6.0270999999999998E-2</v>
       </c>
       <c r="K99" s="6">
-        <v>6.2130999999999999E-2</v>
+        <v>6.2229E-2</v>
       </c>
       <c r="L99" s="1"/>
       <c r="M99" s="1">
         <f>AVERAGE(J99,K99)</f>
-        <v>6.1149999999999996E-2</v>
+        <v>6.1249999999999999E-2</v>
       </c>
       <c r="N99" s="1"/>
       <c r="O99" s="9">
         <f t="shared" si="26"/>
-        <v>6.1149999999999996E-2</v>
+        <v>6.1249999999999999E-2</v>
       </c>
       <c r="P99" s="1"/>
       <c r="Q99" s="1">
         <f>O89/O99</f>
-        <v>14.223385118560918</v>
+        <v>14.200163265306124</v>
       </c>
       <c r="R99" s="15">
         <f t="shared" si="27"/>
-        <v>7.0306751287711536E-2</v>
+        <v>7.04217255334805E-2</v>
       </c>
     </row>
     <row r="100" spans="2:18" x14ac:dyDescent="0.25">
@@ -3693,29 +3693,29 @@
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="6">
-        <v>6.8520999999999999E-2</v>
+        <v>0.68630000000000002</v>
       </c>
       <c r="K100" s="6">
-        <v>7.0539000000000004E-2</v>
+        <v>7.0643999999999998E-2</v>
       </c>
       <c r="L100" s="1"/>
       <c r="M100" s="1">
         <f>AVERAGE(J100,K100)</f>
-        <v>6.9530000000000008E-2</v>
+        <v>0.37847200000000003</v>
       </c>
       <c r="N100" s="1"/>
       <c r="O100" s="9">
         <f t="shared" si="26"/>
-        <v>6.9530000000000008E-2</v>
+        <v>0.37847200000000003</v>
       </c>
       <c r="P100" s="1"/>
       <c r="Q100" s="1">
         <f>O91/O100</f>
-        <v>14.618013806989786</v>
+        <v>2.685510420850155</v>
       </c>
       <c r="R100" s="15">
         <f t="shared" si="27"/>
-        <v>6.8408746441451396E-2</v>
+        <v>0.37236869097064568</v>
       </c>
     </row>
     <row r="101" spans="2:18" x14ac:dyDescent="0.25">
@@ -3734,29 +3734,29 @@
       </c>
       <c r="I101" s="5"/>
       <c r="J101" s="8">
-        <v>4.3298999999999997E-2</v>
+        <v>4.3385E-2</v>
       </c>
       <c r="K101" s="8">
-        <v>4.5069999999999999E-2</v>
+        <v>4.5154E-2</v>
       </c>
       <c r="L101" s="5"/>
       <c r="M101" s="8">
         <f t="shared" ref="M101" si="28">AVERAGE(J101,K101)</f>
-        <v>4.4184500000000002E-2</v>
+        <v>4.4269500000000003E-2</v>
       </c>
       <c r="N101" s="5"/>
       <c r="O101" s="11">
         <f>M101</f>
-        <v>4.4184500000000002E-2</v>
+        <v>4.4269500000000003E-2</v>
       </c>
       <c r="P101" s="1"/>
       <c r="Q101" s="1">
         <f>O93/O101</f>
-        <v>12.889157962633956</v>
+        <v>12.864410033996318</v>
       </c>
       <c r="R101" s="15">
         <f t="shared" si="27"/>
-        <v>7.7584587208802083E-2</v>
+        <v>7.7733840678067295E-2</v>
       </c>
     </row>
     <row r="102" spans="2:18" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
         <v>0.57244349999999999</v>
       </c>
       <c r="N107" s="1"/>
-      <c r="O107" s="26">
+      <c r="O107" s="27">
         <f>SUM(M107,M108,)</f>
         <v>0.7543995</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>0.18195600000000001</v>
       </c>
       <c r="N108" s="1"/>
-      <c r="O108" s="26"/>
+      <c r="O108" s="27"/>
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
       <c r="R108" s="15"/>
@@ -4006,7 +4006,7 @@
         <v>0.62467099999999998</v>
       </c>
       <c r="N109" s="1"/>
-      <c r="O109" s="26">
+      <c r="O109" s="27">
         <f>SUM(M109,M110)</f>
         <v>0.82504650000000002</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>0.20037549999999998</v>
       </c>
       <c r="N110" s="1"/>
-      <c r="O110" s="26"/>
+      <c r="O110" s="27"/>
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
       <c r="R110" s="15"/>
@@ -4073,7 +4073,7 @@
         <v>0.45802799999999999</v>
       </c>
       <c r="N111" s="1"/>
-      <c r="O111" s="26">
+      <c r="O111" s="27">
         <f>SUM(M111:M112)</f>
         <v>0.60003849999999992</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>0.14201049999999998</v>
       </c>
       <c r="N112" s="5"/>
-      <c r="O112" s="27"/>
+      <c r="O112" s="28"/>
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
       <c r="R112" s="15"/>
@@ -4524,7 +4524,7 @@
     </row>
     <row r="126" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B126" s="22"/>
-      <c r="C126" s="28"/>
+      <c r="C126" s="26"/>
       <c r="D126" s="18">
         <v>89</v>
       </c>
@@ -4957,24 +4957,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O69:O70"/>
+    <mergeCell ref="O71:O72"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="O51:O52"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O67:O68"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="O29:O30"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="O13:O14"/>
     <mergeCell ref="O111:O112"/>
     <mergeCell ref="O89:O90"/>
     <mergeCell ref="O91:O92"/>
     <mergeCell ref="O93:O94"/>
     <mergeCell ref="O107:O108"/>
     <mergeCell ref="O109:O110"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="O29:O30"/>
-    <mergeCell ref="O31:O32"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O69:O70"/>
-    <mergeCell ref="O71:O72"/>
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="O51:O52"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="O67:O68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Run CCP 1vs60 finished
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L101" sqref="L101"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K120" sqref="K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,29 +4154,29 @@
       </c>
       <c r="I114" s="3"/>
       <c r="J114" s="3">
-        <v>2.1222000000000001E-2</v>
+        <v>1.3826E-2</v>
       </c>
       <c r="K114" s="3">
-        <v>2.3970999999999999E-2</v>
+        <v>1.5315E-2</v>
       </c>
       <c r="L114" s="3"/>
       <c r="M114" s="3">
         <f>AVERAGE(J114,K114)</f>
-        <v>2.2596499999999999E-2</v>
+        <v>1.45705E-2</v>
       </c>
       <c r="N114" s="3"/>
       <c r="O114" s="10">
         <f>M114</f>
-        <v>2.2596499999999999E-2</v>
+        <v>1.45705E-2</v>
       </c>
       <c r="P114" s="1"/>
       <c r="Q114" s="1">
         <f>O104/O114</f>
-        <v>265.17582368950946</v>
+        <v>411.24501561374007</v>
       </c>
       <c r="R114" s="15">
         <f>1/Q114</f>
-        <v>3.7710828464169702E-3</v>
+        <v>2.4316404139454548E-3</v>
       </c>
     </row>
     <row r="115" spans="2:18" x14ac:dyDescent="0.25">
@@ -4277,29 +4277,29 @@
       </c>
       <c r="I117" s="1"/>
       <c r="J117" s="6">
-        <v>5.4769999999999999E-2</v>
+        <v>5.4858999999999998E-2</v>
       </c>
       <c r="K117" s="6">
-        <v>5.6631000000000001E-2</v>
+        <v>5.6715000000000002E-2</v>
       </c>
       <c r="L117" s="1"/>
       <c r="M117" s="1">
         <f>AVERAGE(J117,K117)</f>
-        <v>5.57005E-2</v>
+        <v>5.5787000000000003E-2</v>
       </c>
       <c r="N117" s="1"/>
       <c r="O117" s="9">
         <f t="shared" si="32"/>
-        <v>5.57005E-2</v>
+        <v>5.5787000000000003E-2</v>
       </c>
       <c r="P117" s="1"/>
       <c r="Q117" s="1">
         <f>O107/O117</f>
-        <v>13.543855082090825</v>
+        <v>13.522854786957534</v>
       </c>
       <c r="R117" s="15">
         <f t="shared" si="33"/>
-        <v>7.3834221788323023E-2</v>
+        <v>7.3948882521793824E-2</v>
       </c>
     </row>
     <row r="118" spans="2:18" x14ac:dyDescent="0.25">
@@ -4318,29 +4318,29 @@
       </c>
       <c r="I118" s="1"/>
       <c r="J118" s="6">
-        <v>5.9110999999999997E-2</v>
+        <v>5.9202999999999999E-2</v>
       </c>
       <c r="K118" s="6">
-        <v>6.1005999999999998E-2</v>
+        <v>6.1093000000000001E-2</v>
       </c>
       <c r="L118" s="1"/>
       <c r="M118" s="1">
         <f>AVERAGE(J118,K118)</f>
-        <v>6.0058500000000001E-2</v>
+        <v>6.0148E-2</v>
       </c>
       <c r="N118" s="1"/>
       <c r="O118" s="9">
         <f t="shared" si="32"/>
-        <v>6.0058500000000001E-2</v>
+        <v>6.0148E-2</v>
       </c>
       <c r="P118" s="1"/>
       <c r="Q118" s="1">
         <f>O109/O118</f>
-        <v>13.737381053472864</v>
+        <v>13.716939881625324</v>
       </c>
       <c r="R118" s="15">
         <f t="shared" si="33"/>
-        <v>7.2794078879190441E-2</v>
+        <v>7.2902557613419364E-2</v>
       </c>
     </row>
     <row r="119" spans="2:18" x14ac:dyDescent="0.25">
@@ -4359,29 +4359,29 @@
       </c>
       <c r="I119" s="5"/>
       <c r="J119" s="8">
-        <v>4.539E-2</v>
+        <v>4.5470999999999998E-2</v>
       </c>
       <c r="K119" s="8">
-        <v>4.7148000000000002E-2</v>
+        <v>4.7224000000000002E-2</v>
       </c>
       <c r="L119" s="5"/>
       <c r="M119" s="8">
         <f t="shared" ref="M119" si="34">AVERAGE(J119,K119)</f>
-        <v>4.6269000000000005E-2</v>
+        <v>4.63475E-2</v>
       </c>
       <c r="N119" s="5"/>
       <c r="O119" s="11">
         <f>M119</f>
-        <v>4.6269000000000005E-2</v>
+        <v>4.63475E-2</v>
       </c>
       <c r="P119" s="1"/>
       <c r="Q119" s="6">
         <f>O111/O119</f>
-        <v>12.968477814519437</v>
+        <v>12.946512756890877</v>
       </c>
       <c r="R119" s="15">
         <f t="shared" si="33"/>
-        <v>7.711005210498996E-2</v>
+        <v>7.7240877043723039E-2</v>
       </c>
     </row>
     <row r="120" spans="2:18" x14ac:dyDescent="0.25">
@@ -4957,24 +4957,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O111:O112"/>
+    <mergeCell ref="O89:O90"/>
+    <mergeCell ref="O91:O92"/>
+    <mergeCell ref="O93:O94"/>
+    <mergeCell ref="O107:O108"/>
+    <mergeCell ref="O109:O110"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="O29:O30"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="O13:O14"/>
     <mergeCell ref="O69:O70"/>
     <mergeCell ref="O71:O72"/>
     <mergeCell ref="O49:O50"/>
     <mergeCell ref="O51:O52"/>
     <mergeCell ref="O53:O54"/>
     <mergeCell ref="O67:O68"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="O29:O30"/>
-    <mergeCell ref="O31:O32"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O111:O112"/>
-    <mergeCell ref="O89:O90"/>
-    <mergeCell ref="O91:O92"/>
-    <mergeCell ref="O93:O94"/>
-    <mergeCell ref="O107:O108"/>
-    <mergeCell ref="O109:O110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>